<commit_message>
num weeks standardization + small changes
</commit_message>
<xml_diff>
--- a/tables/monthly_tables/detrended_covar/explained_var_ratio.xlsx
+++ b/tables/monthly_tables/detrended_covar/explained_var_ratio.xlsx
@@ -453,1598 +453,1598 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>0.1239930242300034</v>
+        <v>0.1338727325201035</v>
       </c>
       <c r="B2">
-        <v>0.1235910281538963</v>
+        <v>0.125913679599762</v>
       </c>
       <c r="C2">
-        <v>0.1225515156984329</v>
+        <v>0.1254069656133652</v>
       </c>
       <c r="D2">
-        <v>0.11334078758955</v>
+        <v>0.1135641038417816</v>
       </c>
       <c r="E2">
-        <v>0.09903284907341003</v>
+        <v>0.1006886288523674</v>
       </c>
       <c r="F2">
-        <v>0.1126953586935997</v>
+        <v>0.1153330653905869</v>
       </c>
       <c r="G2">
-        <v>0.123775489628315</v>
+        <v>0.130140632390976</v>
       </c>
       <c r="H2">
-        <v>0.1804162263870239</v>
+        <v>0.1135972961783409</v>
       </c>
       <c r="I2">
-        <v>0.0954827144742012</v>
+        <v>0.09922987967729568</v>
       </c>
       <c r="J2">
-        <v>0.08555404841899872</v>
+        <v>0.08660564571619034</v>
       </c>
       <c r="K2">
-        <v>0.0962747186422348</v>
+        <v>0.0994059219956398</v>
       </c>
       <c r="L2">
-        <v>0.1021358743309975</v>
+        <v>0.1058914437890053</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>0.09759259968996048</v>
+        <v>0.07261680066585541</v>
       </c>
       <c r="B3">
-        <v>0.08096770197153091</v>
+        <v>0.07883117347955704</v>
       </c>
       <c r="C3">
-        <v>0.09077233076095581</v>
+        <v>0.08991431444883347</v>
       </c>
       <c r="D3">
-        <v>0.09410414844751358</v>
+        <v>0.08436419069766998</v>
       </c>
       <c r="E3">
-        <v>0.0747806504368782</v>
+        <v>0.07691492885351181</v>
       </c>
       <c r="F3">
-        <v>0.07588806748390198</v>
+        <v>0.0730605274438858</v>
       </c>
       <c r="G3">
-        <v>0.1130421832203865</v>
+        <v>0.09675819426774979</v>
       </c>
       <c r="H3">
-        <v>0.09386274218559265</v>
+        <v>0.1048085913062096</v>
       </c>
       <c r="I3">
-        <v>0.08588337898254395</v>
+        <v>0.08888678252696991</v>
       </c>
       <c r="J3">
-        <v>0.06677331030368805</v>
+        <v>0.06197302043437958</v>
       </c>
       <c r="K3">
-        <v>0.08252730965614319</v>
+        <v>0.0785071924328804</v>
       </c>
       <c r="L3">
-        <v>0.08523058891296387</v>
+        <v>0.06644423305988312</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>0.06571836024522781</v>
+        <v>0.05996358394622803</v>
       </c>
       <c r="B4">
-        <v>0.07276236265897751</v>
+        <v>0.07267205417156219</v>
       </c>
       <c r="C4">
-        <v>0.07455824315547943</v>
+        <v>0.07124143838882446</v>
       </c>
       <c r="D4">
-        <v>0.07652457058429718</v>
+        <v>0.06932410597801208</v>
       </c>
       <c r="E4">
-        <v>0.07170435041189194</v>
+        <v>0.06020419299602509</v>
       </c>
       <c r="F4">
-        <v>0.05681236833333969</v>
+        <v>0.05449477210640907</v>
       </c>
       <c r="G4">
-        <v>0.08746735751628876</v>
+        <v>0.08448421955108643</v>
       </c>
       <c r="H4">
-        <v>0.08294189721345901</v>
+        <v>0.07690112292766571</v>
       </c>
       <c r="I4">
-        <v>0.06409239023923874</v>
+        <v>0.06306380033493042</v>
       </c>
       <c r="J4">
-        <v>0.06005566194653511</v>
+        <v>0.05895973742008209</v>
       </c>
       <c r="K4">
-        <v>0.07305909693241119</v>
+        <v>0.07013998925685883</v>
       </c>
       <c r="L4">
-        <v>0.06451541930437088</v>
+        <v>0.06244392320513725</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>0.05322761461138725</v>
+        <v>0.05181236192584038</v>
       </c>
       <c r="B5">
-        <v>0.05109285935759544</v>
+        <v>0.05125131085515022</v>
       </c>
       <c r="C5">
-        <v>0.04987461492419243</v>
+        <v>0.05191419646143913</v>
       </c>
       <c r="D5">
-        <v>0.0516803190112114</v>
+        <v>0.0520835667848587</v>
       </c>
       <c r="E5">
-        <v>0.05634116381406784</v>
+        <v>0.05191752687096596</v>
       </c>
       <c r="F5">
-        <v>0.05286325886845589</v>
+        <v>0.05335304513573647</v>
       </c>
       <c r="G5">
-        <v>0.07286342978477478</v>
+        <v>0.05007528141140938</v>
       </c>
       <c r="H5">
-        <v>0.06678962707519531</v>
+        <v>0.06451497226953506</v>
       </c>
       <c r="I5">
-        <v>0.05510633066296577</v>
+        <v>0.05422381311655045</v>
       </c>
       <c r="J5">
-        <v>0.05178260430693626</v>
+        <v>0.0564587265253067</v>
       </c>
       <c r="K5">
-        <v>0.06017611175775528</v>
+        <v>0.05445414036512375</v>
       </c>
       <c r="L5">
-        <v>0.05918483808636665</v>
+        <v>0.06021403148770332</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>0.04778000712394714</v>
+        <v>0.04734945297241211</v>
       </c>
       <c r="B6">
-        <v>0.04796347394585609</v>
+        <v>0.04718491807579994</v>
       </c>
       <c r="C6">
-        <v>0.04646819084882736</v>
+        <v>0.04352777078747749</v>
       </c>
       <c r="D6">
-        <v>0.04688562080264091</v>
+        <v>0.04469393938779831</v>
       </c>
       <c r="E6">
-        <v>0.04592891782522202</v>
+        <v>0.04704675450921059</v>
       </c>
       <c r="F6">
-        <v>0.04891319572925568</v>
+        <v>0.04945943504571915</v>
       </c>
       <c r="G6">
-        <v>0.04602906480431557</v>
+        <v>0.04439662396907806</v>
       </c>
       <c r="H6">
-        <v>0.04993301257491112</v>
+        <v>0.04725673794746399</v>
       </c>
       <c r="I6">
-        <v>0.05126562342047691</v>
+        <v>0.05093162879347801</v>
       </c>
       <c r="J6">
-        <v>0.04960191622376442</v>
+        <v>0.05174275860190392</v>
       </c>
       <c r="K6">
-        <v>0.05183997377753258</v>
+        <v>0.04552011936903</v>
       </c>
       <c r="L6">
-        <v>0.05167658254504204</v>
+        <v>0.0503842905163765</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>0.04413731396198273</v>
+        <v>0.03926332667469978</v>
       </c>
       <c r="B7">
-        <v>0.03963686898350716</v>
+        <v>0.03933484107255936</v>
       </c>
       <c r="C7">
-        <v>0.04213923588395119</v>
+        <v>0.04087380692362785</v>
       </c>
       <c r="D7">
-        <v>0.04072258248925209</v>
+        <v>0.04106708988547325</v>
       </c>
       <c r="E7">
-        <v>0.04385783523321152</v>
+        <v>0.04564728587865829</v>
       </c>
       <c r="F7">
-        <v>0.04731365665793419</v>
+        <v>0.04507629200816154</v>
       </c>
       <c r="G7">
-        <v>0.04202990606427193</v>
+        <v>0.04034591838717461</v>
       </c>
       <c r="H7">
-        <v>0.04238789156079292</v>
+        <v>0.04318524152040482</v>
       </c>
       <c r="I7">
-        <v>0.04860072582960129</v>
+        <v>0.04617078974843025</v>
       </c>
       <c r="J7">
-        <v>0.04140601307153702</v>
+        <v>0.04378877952694893</v>
       </c>
       <c r="K7">
-        <v>0.04254665598273277</v>
+        <v>0.03884269669651985</v>
       </c>
       <c r="L7">
-        <v>0.04731765016913414</v>
+        <v>0.04242680221796036</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>0.03609642013907433</v>
+        <v>0.0351327657699585</v>
       </c>
       <c r="B8">
-        <v>0.03649822995066643</v>
+        <v>0.03650553897023201</v>
       </c>
       <c r="C8">
-        <v>0.03933171927928925</v>
+        <v>0.03660107403993607</v>
       </c>
       <c r="D8">
-        <v>0.03782433643937111</v>
+        <v>0.03590208664536476</v>
       </c>
       <c r="E8">
-        <v>0.03961845114827156</v>
+        <v>0.03916233405470848</v>
       </c>
       <c r="F8">
-        <v>0.04046126827597618</v>
+        <v>0.03753549233078957</v>
       </c>
       <c r="G8">
-        <v>0.03483699634671211</v>
+        <v>0.03848766908049583</v>
       </c>
       <c r="H8">
-        <v>0.03628254681825638</v>
+        <v>0.03966401144862175</v>
       </c>
       <c r="I8">
-        <v>0.04450727254152298</v>
+        <v>0.0400247797369957</v>
       </c>
       <c r="J8">
-        <v>0.03795841336250305</v>
+        <v>0.03816371038556099</v>
       </c>
       <c r="K8">
-        <v>0.03674555942416191</v>
+        <v>0.03702622279524803</v>
       </c>
       <c r="L8">
-        <v>0.03945177048444748</v>
+        <v>0.03799231350421906</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>0.03213207796216011</v>
+        <v>0.0339016318321228</v>
       </c>
       <c r="B9">
-        <v>0.03331661969423294</v>
+        <v>0.03322781622409821</v>
       </c>
       <c r="C9">
-        <v>0.03587405383586884</v>
+        <v>0.03489253297448158</v>
       </c>
       <c r="D9">
-        <v>0.03342914581298828</v>
+        <v>0.03463001176714897</v>
       </c>
       <c r="E9">
-        <v>0.03853821381926537</v>
+        <v>0.03837613388895988</v>
       </c>
       <c r="F9">
-        <v>0.03450718522071838</v>
+        <v>0.03596978262066841</v>
       </c>
       <c r="G9">
-        <v>0.03332988172769547</v>
+        <v>0.03513386845588684</v>
       </c>
       <c r="H9">
-        <v>0.03312663361430168</v>
+        <v>0.03891538083553314</v>
       </c>
       <c r="I9">
-        <v>0.03712469711899757</v>
+        <v>0.03455007448792458</v>
       </c>
       <c r="J9">
-        <v>0.03576755151152611</v>
+        <v>0.03403459489345551</v>
       </c>
       <c r="K9">
-        <v>0.03524764999747276</v>
+        <v>0.03620685264468193</v>
       </c>
       <c r="L9">
-        <v>0.03471890836954117</v>
+        <v>0.03490334376692772</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>0.02835508435964584</v>
+        <v>0.03222085162997246</v>
       </c>
       <c r="B10">
-        <v>0.03120493702590466</v>
+        <v>0.03100530058145523</v>
       </c>
       <c r="C10">
-        <v>0.03182140365242958</v>
+        <v>0.03237501531839371</v>
       </c>
       <c r="D10">
-        <v>0.03120905347168446</v>
+        <v>0.032764732837677</v>
       </c>
       <c r="E10">
-        <v>0.03347288444638252</v>
+        <v>0.03147232159972191</v>
       </c>
       <c r="F10">
-        <v>0.03310951590538025</v>
+        <v>0.03404843807220459</v>
       </c>
       <c r="G10">
-        <v>0.03242963925004005</v>
+        <v>0.03183456137776375</v>
       </c>
       <c r="H10">
-        <v>0.03138804063200951</v>
+        <v>0.03400585427880287</v>
       </c>
       <c r="I10">
-        <v>0.03230169788002968</v>
+        <v>0.03240593150258064</v>
       </c>
       <c r="J10">
-        <v>0.0318186953663826</v>
+        <v>0.03331540897488594</v>
       </c>
       <c r="K10">
-        <v>0.03192320838570595</v>
+        <v>0.03267784789204597</v>
       </c>
       <c r="L10">
-        <v>0.03211428597569466</v>
+        <v>0.03160518407821655</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>0.02759090065956116</v>
+        <v>0.02706059440970421</v>
       </c>
       <c r="B11">
-        <v>0.02929168194532394</v>
+        <v>0.02918297052383423</v>
       </c>
       <c r="C11">
-        <v>0.02927660383284092</v>
+        <v>0.03002505004405975</v>
       </c>
       <c r="D11">
-        <v>0.02972429618239403</v>
+        <v>0.02894779667258263</v>
       </c>
       <c r="E11">
-        <v>0.02944565936923027</v>
+        <v>0.0306889358907938</v>
       </c>
       <c r="F11">
-        <v>0.03229261934757233</v>
+        <v>0.03169231116771698</v>
       </c>
       <c r="G11">
-        <v>0.02817012742161751</v>
+        <v>0.02915521711111069</v>
       </c>
       <c r="H11">
-        <v>0.02903623878955841</v>
+        <v>0.03169717267155647</v>
       </c>
       <c r="I11">
-        <v>0.03113873489201069</v>
+        <v>0.02926719188690186</v>
       </c>
       <c r="J11">
-        <v>0.03067154437303543</v>
+        <v>0.03150303289294243</v>
       </c>
       <c r="K11">
-        <v>0.02892906405031681</v>
+        <v>0.03036756068468094</v>
       </c>
       <c r="L11">
-        <v>0.02840276993811131</v>
+        <v>0.0302783977240324</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>0.02537295036017895</v>
+        <v>0.02686254866421223</v>
       </c>
       <c r="B12">
-        <v>0.02592997066676617</v>
+        <v>0.02587605081498623</v>
       </c>
       <c r="C12">
-        <v>0.02734733186662197</v>
+        <v>0.02667060494422913</v>
       </c>
       <c r="D12">
-        <v>0.02802945859730244</v>
+        <v>0.02739734388887882</v>
       </c>
       <c r="E12">
-        <v>0.02902908436954021</v>
+        <v>0.02735623717308044</v>
       </c>
       <c r="F12">
-        <v>0.03053722344338894</v>
+        <v>0.02984047308564186</v>
       </c>
       <c r="G12">
-        <v>0.02744080126285553</v>
+        <v>0.02799607627093792</v>
       </c>
       <c r="H12">
-        <v>0.02656996808946133</v>
+        <v>0.03028761595487595</v>
       </c>
       <c r="I12">
-        <v>0.02857443690299988</v>
+        <v>0.02681435830891132</v>
       </c>
       <c r="J12">
-        <v>0.03021465055644512</v>
+        <v>0.02997447736561298</v>
       </c>
       <c r="K12">
-        <v>0.02656101807951927</v>
+        <v>0.02924154512584209</v>
       </c>
       <c r="L12">
-        <v>0.02694471180438995</v>
+        <v>0.02802326716482639</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>0.02460449747741222</v>
+        <v>0.02552771754562855</v>
       </c>
       <c r="B13">
-        <v>0.02490224875509739</v>
+        <v>0.02554875239729881</v>
       </c>
       <c r="C13">
-        <v>0.02400650642812252</v>
+        <v>0.02532735094428062</v>
       </c>
       <c r="D13">
-        <v>0.02428882569074631</v>
+        <v>0.02631004899740219</v>
       </c>
       <c r="E13">
-        <v>0.02611567825078964</v>
+        <v>0.02497809194028378</v>
       </c>
       <c r="F13">
-        <v>0.02808968722820282</v>
+        <v>0.02740764617919922</v>
       </c>
       <c r="G13">
-        <v>0.02411773055791855</v>
+        <v>0.02491389587521553</v>
       </c>
       <c r="H13">
-        <v>0.02400586195290089</v>
+        <v>0.02651687152683735</v>
       </c>
       <c r="I13">
-        <v>0.0251042228192091</v>
+        <v>0.02580179646611214</v>
       </c>
       <c r="J13">
-        <v>0.02871453575789928</v>
+        <v>0.02679777331650257</v>
       </c>
       <c r="K13">
-        <v>0.02567601948976517</v>
+        <v>0.02786619588732719</v>
       </c>
       <c r="L13">
-        <v>0.02639170736074448</v>
+        <v>0.02674411423504353</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>0.02374959178268909</v>
+        <v>0.0235342625528574</v>
       </c>
       <c r="B14">
-        <v>0.02300933375954628</v>
+        <v>0.02301761135458946</v>
       </c>
       <c r="C14">
-        <v>0.02384421415627003</v>
+        <v>0.02359144017100334</v>
       </c>
       <c r="D14">
-        <v>0.0236829612404108</v>
+        <v>0.02326559834182262</v>
       </c>
       <c r="E14">
-        <v>0.02374202385544777</v>
+        <v>0.02480421774089336</v>
       </c>
       <c r="F14">
-        <v>0.02660730294883251</v>
+        <v>0.02571313641965389</v>
       </c>
       <c r="G14">
-        <v>0.0231311209499836</v>
+        <v>0.02446543239057064</v>
       </c>
       <c r="H14">
-        <v>0.02273414470255375</v>
+        <v>0.02498333714902401</v>
       </c>
       <c r="I14">
-        <v>0.02464856021106243</v>
+        <v>0.02465181052684784</v>
       </c>
       <c r="J14">
-        <v>0.02650915272533894</v>
+        <v>0.02530659735202789</v>
       </c>
       <c r="K14">
-        <v>0.02410084754228592</v>
+        <v>0.02553184516727924</v>
       </c>
       <c r="L14">
-        <v>0.02420478314161301</v>
+        <v>0.02602857910096645</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>0.02195153012871742</v>
+        <v>0.02311912178993225</v>
       </c>
       <c r="B15">
-        <v>0.02239396423101425</v>
+        <v>0.02214928530156612</v>
       </c>
       <c r="C15">
-        <v>0.02213398180902004</v>
+        <v>0.02284772321581841</v>
       </c>
       <c r="D15">
-        <v>0.0219629742205143</v>
+        <v>0.02300520054996014</v>
       </c>
       <c r="E15">
-        <v>0.02314897812902927</v>
+        <v>0.02390498109161854</v>
       </c>
       <c r="F15">
-        <v>0.02517996542155743</v>
+        <v>0.02438764460384846</v>
       </c>
       <c r="G15">
-        <v>0.02155814319849014</v>
+        <v>0.02369608543813229</v>
       </c>
       <c r="H15">
-        <v>0.02185626327991486</v>
+        <v>0.0245379377156496</v>
       </c>
       <c r="I15">
-        <v>0.02276932075619698</v>
+        <v>0.02344422228634357</v>
       </c>
       <c r="J15">
-        <v>0.02554371580481529</v>
+        <v>0.02483338862657547</v>
       </c>
       <c r="K15">
-        <v>0.02381839789450169</v>
+        <v>0.02338248863816261</v>
       </c>
       <c r="L15">
-        <v>0.02272151224315166</v>
+        <v>0.0234102476388216</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>0.02092991955578327</v>
+        <v>0.0227822121232748</v>
       </c>
       <c r="B16">
-        <v>0.02148278802633286</v>
+        <v>0.02153196558356285</v>
       </c>
       <c r="C16">
-        <v>0.02062848955392838</v>
+        <v>0.02136997319757938</v>
       </c>
       <c r="D16">
-        <v>0.02141279168426991</v>
+        <v>0.02076604589819908</v>
       </c>
       <c r="E16">
-        <v>0.02178723551332951</v>
+        <v>0.02191208861768246</v>
       </c>
       <c r="F16">
-        <v>0.0219537615776062</v>
+        <v>0.02283885143697262</v>
       </c>
       <c r="G16">
-        <v>0.02010401152074337</v>
+        <v>0.02186628989875317</v>
       </c>
       <c r="H16">
-        <v>0.02045637741684914</v>
+        <v>0.0218051802366972</v>
       </c>
       <c r="I16">
-        <v>0.02165996469557285</v>
+        <v>0.02186517231166363</v>
       </c>
       <c r="J16">
-        <v>0.02447018399834633</v>
+        <v>0.02340684272348881</v>
       </c>
       <c r="K16">
-        <v>0.02248436212539673</v>
+        <v>0.0213842149823904</v>
       </c>
       <c r="L16">
-        <v>0.02165046334266663</v>
+        <v>0.02274024672806263</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>0.02024908177554607</v>
+        <v>0.02197181433439255</v>
       </c>
       <c r="B17">
-        <v>0.02076270990073681</v>
+        <v>0.02081560529768467</v>
       </c>
       <c r="C17">
-        <v>0.01979946158826351</v>
+        <v>0.01956178434193134</v>
       </c>
       <c r="D17">
-        <v>0.01939286105334759</v>
+        <v>0.02022920735180378</v>
       </c>
       <c r="E17">
-        <v>0.02146206051111221</v>
+        <v>0.02141768857836723</v>
       </c>
       <c r="F17">
-        <v>0.02134144492447376</v>
+        <v>0.02210044860839844</v>
       </c>
       <c r="G17">
-        <v>0.01966253481805325</v>
+        <v>0.02091233618557453</v>
       </c>
       <c r="H17">
-        <v>0.0193929597735405</v>
+        <v>0.02170257829129696</v>
       </c>
       <c r="I17">
-        <v>0.02118317410349846</v>
+        <v>0.02101203054189682</v>
       </c>
       <c r="J17">
-        <v>0.02334228344261646</v>
+        <v>0.02315941825509071</v>
       </c>
       <c r="K17">
-        <v>0.02020539343357086</v>
+        <v>0.02074450999498367</v>
       </c>
       <c r="L17">
-        <v>0.02052636444568634</v>
+        <v>0.02158032916486263</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>0.01999573037028313</v>
+        <v>0.02059073001146317</v>
       </c>
       <c r="B18">
-        <v>0.02032901905477047</v>
+        <v>0.02009419724345207</v>
       </c>
       <c r="C18">
-        <v>0.01930011063814163</v>
+        <v>0.01939327456057072</v>
       </c>
       <c r="D18">
-        <v>0.01871877908706665</v>
+        <v>0.01957697235047817</v>
       </c>
       <c r="E18">
-        <v>0.02061383984982967</v>
+        <v>0.02051487006247044</v>
       </c>
       <c r="F18">
-        <v>0.02097731083631516</v>
+        <v>0.02189897559583187</v>
       </c>
       <c r="G18">
-        <v>0.0178190041333437</v>
+        <v>0.01971432566642761</v>
       </c>
       <c r="H18">
-        <v>0.01786874607205391</v>
+        <v>0.01914337649941444</v>
       </c>
       <c r="I18">
-        <v>0.02023688144981861</v>
+        <v>0.02035017684102058</v>
       </c>
       <c r="J18">
-        <v>0.02194264158606529</v>
+        <v>0.02133136801421642</v>
       </c>
       <c r="K18">
-        <v>0.01930012740194798</v>
+        <v>0.01987983286380768</v>
       </c>
       <c r="L18">
-        <v>0.01982150413095951</v>
+        <v>0.02030050568282604</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>0.01927433349192142</v>
+        <v>0.02013366483151913</v>
       </c>
       <c r="B19">
-        <v>0.01793470792472363</v>
+        <v>0.01791338808834553</v>
       </c>
       <c r="C19">
-        <v>0.01898935623466969</v>
+        <v>0.01820914074778557</v>
       </c>
       <c r="D19">
-        <v>0.0182330496609211</v>
+        <v>0.01905861124396324</v>
       </c>
       <c r="E19">
-        <v>0.01890826597809792</v>
+        <v>0.01994836516678333</v>
       </c>
       <c r="F19">
-        <v>0.01985165663063526</v>
+        <v>0.02083017490804195</v>
       </c>
       <c r="G19">
-        <v>0.01723604276776314</v>
+        <v>0.01911592297255993</v>
       </c>
       <c r="H19">
-        <v>0.01605451107025146</v>
+        <v>0.01818354055285454</v>
       </c>
       <c r="I19">
-        <v>0.018741425126791</v>
+        <v>0.01939662359654903</v>
       </c>
       <c r="J19">
-        <v>0.02121313475072384</v>
+        <v>0.02112765423953533</v>
       </c>
       <c r="K19">
-        <v>0.01880237460136414</v>
+        <v>0.0195916797965765</v>
       </c>
       <c r="L19">
-        <v>0.01925056800246239</v>
+        <v>0.01990029588341713</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>0.01857995986938477</v>
+        <v>0.01849491335451603</v>
       </c>
       <c r="B20">
-        <v>0.01747834496200085</v>
+        <v>0.01766425371170044</v>
       </c>
       <c r="C20">
-        <v>0.01797029748558998</v>
+        <v>0.01802777498960495</v>
       </c>
       <c r="D20">
-        <v>0.01780118048191071</v>
+        <v>0.01871654950082302</v>
       </c>
       <c r="E20">
-        <v>0.01876848563551903</v>
+        <v>0.01893363893032074</v>
       </c>
       <c r="F20">
-        <v>0.01868714950978756</v>
+        <v>0.01932000182569027</v>
       </c>
       <c r="G20">
-        <v>0.01681282743811607</v>
+        <v>0.01721378043293953</v>
       </c>
       <c r="H20">
-        <v>0.0155442738905549</v>
+        <v>0.01792038045823574</v>
       </c>
       <c r="I20">
-        <v>0.01837198995053768</v>
+        <v>0.01875429227948189</v>
       </c>
       <c r="J20">
-        <v>0.0205030981451273</v>
+        <v>0.02049494348466396</v>
       </c>
       <c r="K20">
-        <v>0.01813575252890587</v>
+        <v>0.01899986527860165</v>
       </c>
       <c r="L20">
-        <v>0.01844814792275429</v>
+        <v>0.0184646975249052</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>0.01782353222370148</v>
+        <v>0.01806804724037647</v>
       </c>
       <c r="B21">
-        <v>0.01695779524743557</v>
+        <v>0.01679598540067673</v>
       </c>
       <c r="C21">
-        <v>0.01647945120930672</v>
+        <v>0.0165567509829998</v>
       </c>
       <c r="D21">
-        <v>0.01743178814649582</v>
+        <v>0.01811051368713379</v>
       </c>
       <c r="E21">
-        <v>0.0178306307643652</v>
+        <v>0.01849042437970638</v>
       </c>
       <c r="F21">
-        <v>0.01764396764338017</v>
+        <v>0.01833630912005901</v>
       </c>
       <c r="G21">
-        <v>0.01567449048161507</v>
+        <v>0.01670115627348423</v>
       </c>
       <c r="H21">
-        <v>0.01528904959559441</v>
+        <v>0.01706064864993095</v>
       </c>
       <c r="I21">
-        <v>0.01753027550876141</v>
+        <v>0.01790322735905647</v>
       </c>
       <c r="J21">
-        <v>0.01922427304089069</v>
+        <v>0.01950682327151299</v>
       </c>
       <c r="K21">
-        <v>0.01755795441567898</v>
+        <v>0.0181496050208807</v>
       </c>
       <c r="L21">
-        <v>0.01772459037601948</v>
+        <v>0.01805507205426693</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22">
-        <v>0.01664756052196026</v>
+        <v>0.01781157776713371</v>
       </c>
       <c r="B22">
-        <v>0.01651286147534847</v>
+        <v>0.01647081971168518</v>
       </c>
       <c r="C22">
-        <v>0.01610842347145081</v>
+        <v>0.01630770228803158</v>
       </c>
       <c r="D22">
-        <v>0.01682926900684834</v>
+        <v>0.01747447438538074</v>
       </c>
       <c r="E22">
-        <v>0.01704124175012112</v>
+        <v>0.01749840565025806</v>
       </c>
       <c r="F22">
-        <v>0.01698355004191399</v>
+        <v>0.01724046841263771</v>
       </c>
       <c r="G22">
-        <v>0.01517039351165295</v>
+        <v>0.01651702076196671</v>
       </c>
       <c r="H22">
-        <v>0.01357781235128641</v>
+        <v>0.01541793160140514</v>
       </c>
       <c r="I22">
-        <v>0.01663978025317192</v>
+        <v>0.01721618324518204</v>
       </c>
       <c r="J22">
-        <v>0.01887951791286469</v>
+        <v>0.01853544823825359</v>
       </c>
       <c r="K22">
-        <v>0.01732552796602249</v>
+        <v>0.01736951805651188</v>
       </c>
       <c r="L22">
-        <v>0.01627781428396702</v>
+        <v>0.0174203235656023</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23">
-        <v>0.016055503860116</v>
+        <v>0.01693591848015785</v>
       </c>
       <c r="B23">
-        <v>0.01642093248665333</v>
+        <v>0.01631209440529346</v>
       </c>
       <c r="C23">
-        <v>0.01569616049528122</v>
+        <v>0.0157068595290184</v>
       </c>
       <c r="D23">
-        <v>0.01637757010757923</v>
+        <v>0.0169783029705286</v>
       </c>
       <c r="E23">
-        <v>0.01674810796976089</v>
+        <v>0.01742576994001865</v>
       </c>
       <c r="F23">
-        <v>0.01634527556598186</v>
+        <v>0.01675828918814659</v>
       </c>
       <c r="G23">
-        <v>0.01457614544779062</v>
+        <v>0.01553167682141066</v>
       </c>
       <c r="H23">
-        <v>0.01255927793681622</v>
+        <v>0.01460942905396223</v>
       </c>
       <c r="I23">
-        <v>0.01589333452284336</v>
+        <v>0.0165436640381813</v>
       </c>
       <c r="J23">
-        <v>0.0180596187710762</v>
+        <v>0.01777249947190285</v>
       </c>
       <c r="K23">
-        <v>0.01666660606861115</v>
+        <v>0.01699396036565304</v>
       </c>
       <c r="L23">
-        <v>0.01585416309535503</v>
+        <v>0.01664020493626595</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24">
-        <v>0.01550889015197754</v>
+        <v>0.01594242267310619</v>
       </c>
       <c r="B24">
-        <v>0.01594982855021954</v>
+        <v>0.01599110476672649</v>
       </c>
       <c r="C24">
-        <v>0.01522140577435493</v>
+        <v>0.01530432235449553</v>
       </c>
       <c r="D24">
-        <v>0.01540516968816519</v>
+        <v>0.01618009619414806</v>
       </c>
       <c r="E24">
-        <v>0.01581033505499363</v>
+        <v>0.01647685654461384</v>
       </c>
       <c r="F24">
-        <v>0.01596730388700962</v>
+        <v>0.01655388996005058</v>
       </c>
       <c r="G24">
-        <v>0.01385466940701008</v>
+        <v>0.01528688706457615</v>
       </c>
       <c r="H24">
-        <v>0.01245676726102829</v>
+        <v>0.01406727358698845</v>
       </c>
       <c r="I24">
-        <v>0.01547760143876076</v>
+        <v>0.01553751900792122</v>
       </c>
       <c r="J24">
-        <v>0.0169121827930212</v>
+        <v>0.01652782782912254</v>
       </c>
       <c r="K24">
-        <v>0.01587305590510368</v>
+        <v>0.0162002369761467</v>
       </c>
       <c r="L24">
-        <v>0.01505071762949228</v>
+        <v>0.01579614169895649</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25">
-        <v>0.01437227241694927</v>
+        <v>0.01521469838917255</v>
       </c>
       <c r="B25">
-        <v>0.01528560277074575</v>
+        <v>0.01523143518716097</v>
       </c>
       <c r="C25">
-        <v>0.01419670879840851</v>
+        <v>0.01528398599475622</v>
       </c>
       <c r="D25">
-        <v>0.01468593627214432</v>
+        <v>0.01552731916308403</v>
       </c>
       <c r="E25">
-        <v>0.01544771436601877</v>
+        <v>0.01588810794055462</v>
       </c>
       <c r="F25">
-        <v>0.01498164515942335</v>
+        <v>0.01547235809266567</v>
       </c>
       <c r="G25">
-        <v>0.01345019228756428</v>
+        <v>0.01463638059794903</v>
       </c>
       <c r="H25">
-        <v>0.01132696587592363</v>
+        <v>0.01355749368667603</v>
       </c>
       <c r="I25">
-        <v>0.01492766756564379</v>
+        <v>0.01526197791099548</v>
       </c>
       <c r="J25">
-        <v>0.01624784432351589</v>
+        <v>0.01624478399753571</v>
       </c>
       <c r="K25">
-        <v>0.01571978442370892</v>
+        <v>0.01595295965671539</v>
       </c>
       <c r="L25">
-        <v>0.01467554271221161</v>
+        <v>0.01535311713814735</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26">
-        <v>0.01382352225482464</v>
+        <v>0.014626226387918</v>
       </c>
       <c r="B26">
-        <v>0.01404933165758848</v>
+        <v>0.01483239699155092</v>
       </c>
       <c r="C26">
-        <v>0.01372109819203615</v>
+        <v>0.01442141178995371</v>
       </c>
       <c r="D26">
-        <v>0.01458187494426966</v>
+        <v>0.01497383788228035</v>
       </c>
       <c r="E26">
-        <v>0.01473832968622446</v>
+        <v>0.01534202136099339</v>
       </c>
       <c r="F26">
-        <v>0.0145140802487731</v>
+        <v>0.01473985053598881</v>
       </c>
       <c r="G26">
-        <v>0.01267641875892878</v>
+        <v>0.01383868977427483</v>
       </c>
       <c r="H26">
-        <v>0.01079491246491671</v>
+        <v>0.01207165978848934</v>
       </c>
       <c r="I26">
-        <v>0.01442348212003708</v>
+        <v>0.01457644067704678</v>
       </c>
       <c r="J26">
-        <v>0.01536595076322556</v>
+        <v>0.01565666124224663</v>
       </c>
       <c r="K26">
-        <v>0.01506624557077885</v>
+        <v>0.01564572378993034</v>
       </c>
       <c r="L26">
-        <v>0.01405754964798689</v>
+        <v>0.01505765784531832</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27">
-        <v>0.01332345511764288</v>
+        <v>0.01419575046747923</v>
       </c>
       <c r="B27">
-        <v>0.01361346896737814</v>
+        <v>0.01358369924128056</v>
       </c>
       <c r="C27">
-        <v>0.0128813311457634</v>
+        <v>0.01306109596043825</v>
       </c>
       <c r="D27">
-        <v>0.01373999193310738</v>
+        <v>0.01443131919950247</v>
       </c>
       <c r="E27">
-        <v>0.01442188583314419</v>
+        <v>0.01520273182541132</v>
       </c>
       <c r="F27">
-        <v>0.01326629891991615</v>
+        <v>0.01351428963243961</v>
       </c>
       <c r="G27">
-        <v>0.01217913813889027</v>
+        <v>0.01247220486402512</v>
       </c>
       <c r="H27">
-        <v>0.0099426144734025</v>
+        <v>0.01145222596824169</v>
       </c>
       <c r="I27">
-        <v>0.01441094931215048</v>
+        <v>0.01418257225304842</v>
       </c>
       <c r="J27">
-        <v>0.01513562258332968</v>
+        <v>0.01528591476380825</v>
       </c>
       <c r="K27">
-        <v>0.01389226410537958</v>
+        <v>0.0147757101804018</v>
       </c>
       <c r="L27">
-        <v>0.01319787465035915</v>
+        <v>0.01465476863086224</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28">
-        <v>0.01282898522913456</v>
+        <v>0.013718631118536</v>
       </c>
       <c r="B28">
-        <v>0.01356640830636024</v>
+        <v>0.01344456151127815</v>
       </c>
       <c r="C28">
-        <v>0.01240125950425863</v>
+        <v>0.0125372689217329</v>
       </c>
       <c r="D28">
-        <v>0.01317807473242283</v>
+        <v>0.01409287378191948</v>
       </c>
       <c r="E28">
-        <v>0.01377895288169384</v>
+        <v>0.01470145490020514</v>
       </c>
       <c r="F28">
-        <v>0.01295825839042664</v>
+        <v>0.01320374384522438</v>
       </c>
       <c r="G28">
-        <v>0.01122131384909153</v>
+        <v>0.01198144350200891</v>
       </c>
       <c r="H28">
-        <v>0.009613772854208946</v>
+        <v>0.01126179657876492</v>
       </c>
       <c r="I28">
-        <v>0.01386805810034275</v>
+        <v>0.01408970262855291</v>
       </c>
       <c r="J28">
-        <v>0.01512337103486061</v>
+        <v>0.01478192117065191</v>
       </c>
       <c r="K28">
-        <v>0.0137485833838582</v>
+        <v>0.01411791518330574</v>
       </c>
       <c r="L28">
-        <v>0.0129668889567256</v>
+        <v>0.01442981604486704</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29">
-        <v>0.01253811735659838</v>
+        <v>0.01310729887336493</v>
       </c>
       <c r="B29">
-        <v>0.01312099024653435</v>
+        <v>0.01311674062162638</v>
       </c>
       <c r="C29">
-        <v>0.01204238086938858</v>
+        <v>0.01230484433472157</v>
       </c>
       <c r="D29">
-        <v>0.01266306266188622</v>
+        <v>0.01358349155634642</v>
       </c>
       <c r="E29">
-        <v>0.01367966085672379</v>
+        <v>0.01418054290115833</v>
       </c>
       <c r="F29">
-        <v>0.01278519723564386</v>
+        <v>0.01262332499027252</v>
       </c>
       <c r="G29">
-        <v>0.01036758441478014</v>
+        <v>0.01130457129329443</v>
       </c>
       <c r="H29">
-        <v>0.008789874613285065</v>
+        <v>0.01071085594594479</v>
       </c>
       <c r="I29">
-        <v>0.01267941202968359</v>
+        <v>0.01319137308746576</v>
       </c>
       <c r="J29">
-        <v>0.01445534732192755</v>
+        <v>0.01439712475985289</v>
       </c>
       <c r="K29">
-        <v>0.01363113429397345</v>
+        <v>0.01379486359655857</v>
       </c>
       <c r="L29">
-        <v>0.01264494843780994</v>
+        <v>0.01334571279585361</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30">
-        <v>0.01192716136574745</v>
+        <v>0.01292108837515116</v>
       </c>
       <c r="B30">
-        <v>0.01251287572085857</v>
+        <v>0.01261907257139683</v>
       </c>
       <c r="C30">
-        <v>0.01166297495365143</v>
+        <v>0.01161875762045383</v>
       </c>
       <c r="D30">
-        <v>0.01249241922050714</v>
+        <v>0.01267289556562901</v>
       </c>
       <c r="E30">
-        <v>0.01270755752921104</v>
+        <v>0.01331024710088968</v>
       </c>
       <c r="F30">
-        <v>0.01213953830301762</v>
+        <v>0.01214020140469074</v>
       </c>
       <c r="G30">
-        <v>0.009986496530473232</v>
+        <v>0.01071824878454208</v>
       </c>
       <c r="H30">
-        <v>0.008199225179851055</v>
+        <v>0.01035148277878761</v>
       </c>
       <c r="I30">
-        <v>0.01234917622059584</v>
+        <v>0.01284029427915812</v>
       </c>
       <c r="J30">
-        <v>0.01402048952877522</v>
+        <v>0.01427466794848442</v>
       </c>
       <c r="K30">
-        <v>0.01246249675750732</v>
+        <v>0.0130575904622674</v>
       </c>
       <c r="L30">
-        <v>0.01234832406044006</v>
+        <v>0.01296994090080261</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31">
-        <v>0.01151207834482193</v>
+        <v>0.0123857157304883</v>
       </c>
       <c r="B31">
-        <v>0.01228844840079546</v>
+        <v>0.01227681897580624</v>
       </c>
       <c r="C31">
-        <v>0.01131697650998831</v>
+        <v>0.01150182168930769</v>
       </c>
       <c r="D31">
-        <v>0.01197143737226725</v>
+        <v>0.01254683639854193</v>
       </c>
       <c r="E31">
-        <v>0.01209056749939919</v>
+        <v>0.01262989733368158</v>
       </c>
       <c r="F31">
-        <v>0.01206833682954311</v>
+        <v>0.01169313117861748</v>
       </c>
       <c r="G31">
-        <v>0.009497110731899738</v>
+        <v>0.01030728127807379</v>
       </c>
       <c r="H31">
-        <v>0.007930539548397064</v>
+        <v>0.00905653927475214</v>
       </c>
       <c r="I31">
-        <v>0.01227262243628502</v>
+        <v>0.01246047671884298</v>
       </c>
       <c r="J31">
-        <v>0.01369291450828314</v>
+        <v>0.01405965443700552</v>
       </c>
       <c r="K31">
-        <v>0.01222949475049973</v>
+        <v>0.01263730227947235</v>
       </c>
       <c r="L31">
-        <v>0.01193422172218561</v>
+        <v>0.01241208240389824</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32">
-        <v>0.01135813351720572</v>
+        <v>0.01213699579238892</v>
       </c>
       <c r="B32">
-        <v>0.01196081377565861</v>
+        <v>0.01185929961502552</v>
       </c>
       <c r="C32">
-        <v>0.01097127888351679</v>
+        <v>0.01111058704555035</v>
       </c>
       <c r="D32">
-        <v>0.01127977669239044</v>
+        <v>0.01161486189812422</v>
       </c>
       <c r="E32">
-        <v>0.0115061504766345</v>
+        <v>0.0122300498187542</v>
       </c>
       <c r="F32">
-        <v>0.01141070201992989</v>
+        <v>0.01143319997936487</v>
       </c>
       <c r="G32">
-        <v>0.008752420544624329</v>
+        <v>0.009905739687383175</v>
       </c>
       <c r="H32">
-        <v>0.007371945306658745</v>
+        <v>0.008501225151121616</v>
       </c>
       <c r="I32">
-        <v>0.01148976385593414</v>
+        <v>0.01205092389136553</v>
       </c>
       <c r="J32">
-        <v>0.01315918657928705</v>
+        <v>0.0131826139986515</v>
       </c>
       <c r="K32">
-        <v>0.01193472277373075</v>
+        <v>0.01226294133812189</v>
       </c>
       <c r="L32">
-        <v>0.01135705597698689</v>
+        <v>0.01222090143710375</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33">
-        <v>0.01098267361521721</v>
+        <v>0.01162144169211388</v>
       </c>
       <c r="B33">
-        <v>0.01166847441345453</v>
+        <v>0.01180180441588163</v>
       </c>
       <c r="C33">
-        <v>0.01046273298561573</v>
+        <v>0.01090835314244032</v>
       </c>
       <c r="D33">
-        <v>0.01039351336658001</v>
+        <v>0.01125151757150888</v>
       </c>
       <c r="E33">
-        <v>0.0113685205578804</v>
+        <v>0.01150191482156515</v>
       </c>
       <c r="F33">
-        <v>0.01067104935646057</v>
+        <v>0.01104834489524364</v>
       </c>
       <c r="G33">
-        <v>0.008409508503973484</v>
+        <v>0.009626044891774654</v>
       </c>
       <c r="H33">
-        <v>0.00718708848580718</v>
+        <v>0.008199214935302734</v>
       </c>
       <c r="I33">
-        <v>0.01117622945457697</v>
+        <v>0.01161912176758051</v>
       </c>
       <c r="J33">
-        <v>0.01277747936546803</v>
+        <v>0.01261330582201481</v>
       </c>
       <c r="K33">
-        <v>0.01165230758488178</v>
+        <v>0.01174215413630009</v>
       </c>
       <c r="L33">
-        <v>0.01110430527478456</v>
+        <v>0.01191827561706305</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>0.0103547153994441</v>
+        <v>0.01131583284586668</v>
       </c>
       <c r="B34">
-        <v>0.01123103685677052</v>
+        <v>0.01135042309761047</v>
       </c>
       <c r="C34">
-        <v>0.01009195949882269</v>
+        <v>0.01084571331739426</v>
       </c>
       <c r="D34">
-        <v>0.010271898470819</v>
+        <v>0.01068673748522997</v>
       </c>
       <c r="E34">
-        <v>0.01092841010540724</v>
+        <v>0.01139800436794758</v>
       </c>
       <c r="F34">
-        <v>0.01039689127355814</v>
+        <v>0.01038925722241402</v>
       </c>
       <c r="G34">
-        <v>0.008106349036097527</v>
+        <v>0.00877098273485899</v>
       </c>
       <c r="H34">
-        <v>0.006213060114532709</v>
+        <v>0.007357378955930471</v>
       </c>
       <c r="I34">
-        <v>0.01065352465957403</v>
+        <v>0.01105201058089733</v>
       </c>
       <c r="J34">
-        <v>0.01213290076702833</v>
+        <v>0.01206321083009243</v>
       </c>
       <c r="K34">
-        <v>0.01132073253393173</v>
+        <v>0.01117938663810492</v>
       </c>
       <c r="L34">
-        <v>0.01103037036955357</v>
+        <v>0.01150178164243698</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35">
-        <v>0.009760776534676552</v>
+        <v>0.0104821128770709</v>
       </c>
       <c r="B35">
-        <v>0.01078420598059893</v>
+        <v>0.01074813678860664</v>
       </c>
       <c r="C35">
-        <v>0.009482145309448242</v>
+        <v>0.009899848140776157</v>
       </c>
       <c r="D35">
-        <v>0.00948621891438961</v>
+        <v>0.01044658478349447</v>
       </c>
       <c r="E35">
-        <v>0.01055728178471327</v>
+        <v>0.01108317635953426</v>
       </c>
       <c r="F35">
-        <v>0.01013064384460449</v>
+        <v>0.01005436852574348</v>
       </c>
       <c r="G35">
-        <v>0.006960612721741199</v>
+        <v>0.008319420740008354</v>
       </c>
       <c r="H35">
-        <v>0.005807495210319757</v>
+        <v>0.006997388321906328</v>
       </c>
       <c r="I35">
-        <v>0.01013368181884289</v>
+        <v>0.01037596724927425</v>
       </c>
       <c r="J35">
-        <v>0.01189382094889879</v>
+        <v>0.01161073241382837</v>
       </c>
       <c r="K35">
-        <v>0.01038266811519861</v>
+        <v>0.01071303896605968</v>
       </c>
       <c r="L35">
-        <v>0.01075225416570902</v>
+        <v>0.01105089019984007</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>0.009448334574699402</v>
+        <v>0.009944981895387173</v>
       </c>
       <c r="B36">
-        <v>0.01012853626161814</v>
+        <v>0.01029569189995527</v>
       </c>
       <c r="C36">
-        <v>0.009407334960997105</v>
+        <v>0.00941824447363615</v>
       </c>
       <c r="D36">
-        <v>0.009289879351854324</v>
+        <v>0.01018671318888664</v>
       </c>
       <c r="E36">
-        <v>0.01035946141928434</v>
+        <v>0.01076070219278336</v>
       </c>
       <c r="F36">
-        <v>0.009536183439195156</v>
+        <v>0.009745310060679913</v>
       </c>
       <c r="G36">
-        <v>0.006820184178650379</v>
+        <v>0.008252592757344246</v>
       </c>
       <c r="H36">
-        <v>0.004633286502212286</v>
+        <v>0.00611509196460247</v>
       </c>
       <c r="I36">
-        <v>0.009689359925687313</v>
+        <v>0.01019783411175013</v>
       </c>
       <c r="J36">
-        <v>0.01109327469021082</v>
+        <v>0.011118502356112</v>
       </c>
       <c r="K36">
-        <v>0.00964156910777092</v>
+        <v>0.01066502928733826</v>
       </c>
       <c r="L36">
-        <v>0.01063771359622478</v>
+        <v>0.01077342312783003</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37">
-        <v>0.009087834507226944</v>
+        <v>0.009422116912901402</v>
       </c>
       <c r="B37">
-        <v>0.009520554915070534</v>
+        <v>0.009532776661217213</v>
       </c>
       <c r="C37">
-        <v>0.008825243450701237</v>
+        <v>0.00900116004049778</v>
       </c>
       <c r="D37">
-        <v>0.009255421347916126</v>
+        <v>0.009436988271772861</v>
       </c>
       <c r="E37">
-        <v>0.01004455611109734</v>
+        <v>0.01012436114251614</v>
       </c>
       <c r="F37">
-        <v>0.009363772347569466</v>
+        <v>0.009606944397091866</v>
       </c>
       <c r="G37">
-        <v>0.006087940186262131</v>
+        <v>0.006952146999537945</v>
       </c>
       <c r="H37">
-        <v>0.004451936110854149</v>
+        <v>0.005888469982892275</v>
       </c>
       <c r="I37">
-        <v>0.008923028595745564</v>
+        <v>0.009070970118045807</v>
       </c>
       <c r="J37">
-        <v>0.01075923722237349</v>
+        <v>0.01064382772892714</v>
       </c>
       <c r="K37">
-        <v>0.009549281559884548</v>
+        <v>0.0100942263379693</v>
       </c>
       <c r="L37">
-        <v>0.009595257230103016</v>
+        <v>0.0103760277852416</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38">
-        <v>0.008689578622579575</v>
+        <v>0.009099463932216167</v>
       </c>
       <c r="B38">
-        <v>0.009306443855166435</v>
+        <v>0.009371898137032986</v>
       </c>
       <c r="C38">
-        <v>0.008597998879849911</v>
+        <v>0.00874505378305912</v>
       </c>
       <c r="D38">
-        <v>0.008465315215289593</v>
+        <v>0.009263582527637482</v>
       </c>
       <c r="E38">
-        <v>0.009134132415056229</v>
+        <v>0.009956937283277512</v>
       </c>
       <c r="F38">
-        <v>0.008888245560228825</v>
+        <v>0.009212136268615723</v>
       </c>
       <c r="G38">
-        <v>0.005093154031783342</v>
+        <v>0.006545111071318388</v>
       </c>
       <c r="H38">
-        <v>0.003843990620225668</v>
+        <v>0.005507232621312141</v>
       </c>
       <c r="I38">
-        <v>0.008676426485180855</v>
+        <v>0.008864715695381165</v>
       </c>
       <c r="J38">
-        <v>0.01030673086643219</v>
+        <v>0.01019547693431377</v>
       </c>
       <c r="K38">
-        <v>0.008798041380941868</v>
+        <v>0.00920978095382452</v>
       </c>
       <c r="L38">
-        <v>0.009400498121976852</v>
+        <v>0.01001234352588654</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39">
-        <v>0.007968095131218433</v>
+        <v>0.008837108500301838</v>
       </c>
       <c r="B39">
-        <v>0.008783072233200073</v>
+        <v>0.008825032040476799</v>
       </c>
       <c r="C39">
-        <v>0.008449524641036987</v>
+        <v>0.008586240001022816</v>
       </c>
       <c r="D39">
-        <v>0.008083458989858627</v>
+        <v>0.008792761713266373</v>
       </c>
       <c r="E39">
-        <v>0.008786734193563461</v>
+        <v>0.008942984044551849</v>
       </c>
       <c r="F39">
-        <v>0.007921644486486912</v>
+        <v>0.008375601842999458</v>
       </c>
       <c r="G39">
-        <v>0.004115873947739601</v>
+        <v>0.00463171536102891</v>
       </c>
       <c r="H39">
-        <v>0.003521309467032552</v>
+        <v>0.004457714501768351</v>
       </c>
       <c r="I39">
-        <v>0.008185905404388905</v>
+        <v>0.008157966658473015</v>
       </c>
       <c r="J39">
-        <v>0.009489383548498154</v>
+        <v>0.009997870773077011</v>
       </c>
       <c r="K39">
-        <v>0.008641242980957031</v>
+        <v>0.009166238829493523</v>
       </c>
       <c r="L39">
-        <v>0.009072296321392059</v>
+        <v>0.009700948372483253</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40">
-        <v>0.007605249527841806</v>
+        <v>0.008185033686459064</v>
       </c>
       <c r="B40">
-        <v>0.008302764967083931</v>
+        <v>0.008287000469863415</v>
       </c>
       <c r="C40">
-        <v>0.007894602604210377</v>
+        <v>0.007667024619877338</v>
       </c>
       <c r="D40">
-        <v>0.007640901021659374</v>
+        <v>0.008419496938586235</v>
       </c>
       <c r="E40">
-        <v>0.008584446273744106</v>
+        <v>0.008631521835923195</v>
       </c>
       <c r="F40">
-        <v>0.007469187956303358</v>
+        <v>0.007048069033771753</v>
       </c>
       <c r="G40">
-        <v>0.002974595641717315</v>
+        <v>0.003994588274508715</v>
       </c>
       <c r="H40">
-        <v>0.00313232745975256</v>
+        <v>0.003972521051764488</v>
       </c>
       <c r="I40">
-        <v>0.007980901747941971</v>
+        <v>0.008091810159385204</v>
       </c>
       <c r="J40">
-        <v>0.009025340899825096</v>
+        <v>0.009464239701628685</v>
       </c>
       <c r="K40">
-        <v>0.008075855672359467</v>
+        <v>0.008665004745125771</v>
       </c>
       <c r="L40">
-        <v>0.008289854042232037</v>
+        <v>0.0086101358756423</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41">
-        <v>0.00705253379419446</v>
+        <v>0.00781644880771637</v>
       </c>
       <c r="B41">
-        <v>0.007486692164093256</v>
+        <v>0.007532502524554729</v>
       </c>
       <c r="C41">
-        <v>0.007401412352919579</v>
+        <v>0.007441720925271511</v>
       </c>
       <c r="D41">
-        <v>0.00750920083373785</v>
+        <v>0.007661668583750725</v>
       </c>
       <c r="E41">
-        <v>0.008138697594404221</v>
+        <v>0.008334657177329063</v>
       </c>
       <c r="F41">
-        <v>0.006476230919361115</v>
+        <v>0.006450464017689228</v>
       </c>
       <c r="G41">
-        <v>0.002169062616303563</v>
+        <v>0.002999757416546345</v>
       </c>
       <c r="H41">
-        <v>0.002708788029849529</v>
+        <v>0.003759237704798579</v>
       </c>
       <c r="I41">
-        <v>0.00582527881488204</v>
+        <v>0.005870094057172537</v>
       </c>
       <c r="J41">
-        <v>0.008402426727116108</v>
+        <v>0.009089017286896706</v>
       </c>
       <c r="K41">
-        <v>0.007476859726011753</v>
+        <v>0.007836080156266689</v>
       </c>
       <c r="L41">
-        <v>0.007319312542676926</v>
+        <v>0.007924188859760761</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42">
-        <v>-7.392268288925093E-18</v>
+        <v>1.232081965521101E-17</v>
       </c>
       <c r="B42">
-        <v>1.434028764935001E-17</v>
+        <v>1.596203645162555E-17</v>
       </c>
       <c r="C42">
-        <v>8.361128396796203E-18</v>
+        <v>2.352005022861034E-17</v>
       </c>
       <c r="D42">
-        <v>-6.662650320900244E-18</v>
+        <v>2.498063943214217E-18</v>
       </c>
       <c r="E42">
-        <v>-1.550719795692346E-17</v>
+        <v>1.427093682679356E-17</v>
       </c>
       <c r="F42">
-        <v>-7.084283304272611E-18</v>
+        <v>5.920245794966551E-18</v>
       </c>
       <c r="G42">
-        <v>1.367965902595392E-17</v>
+        <v>1.529889568070913E-18</v>
       </c>
       <c r="H42">
-        <v>9.800834598583522E-18</v>
+        <v>1.689958632574545E-18</v>
       </c>
       <c r="I42">
-        <v>2.507923108935237E-18</v>
+        <v>-5.636845858890065E-18</v>
       </c>
       <c r="J42">
-        <v>7.386348984461663E-18</v>
+        <v>3.049156896305727E-18</v>
       </c>
       <c r="K42">
-        <v>1.228096754086427E-18</v>
+        <v>8.531793955139369E-18</v>
       </c>
       <c r="L42">
-        <v>3.739588919890162E-17</v>
+        <v>5.769029527571192E-19</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43">
-        <v>-7.392268288925093E-18</v>
+        <v>-1.380078639177251E-17</v>
       </c>
       <c r="B43">
-        <v>3.865887787879161E-19</v>
+        <v>5.831454160063578E-18</v>
       </c>
       <c r="C43">
-        <v>-4.805145117879741E-18</v>
+        <v>1.683705291900251E-17</v>
       </c>
       <c r="D43">
-        <v>-1.23711296072471E-17</v>
+        <v>-3.099170469528337E-17</v>
       </c>
       <c r="E43">
-        <v>-1.550719795692346E-17</v>
+        <v>-5.467498929840885E-19</v>
       </c>
       <c r="F43">
-        <v>-1.3981489786849E-17</v>
+        <v>-1.092081233256195E-17</v>
       </c>
       <c r="G43">
-        <v>-1.078290064493404E-17</v>
+        <v>-1.028568320590903E-17</v>
       </c>
       <c r="H43">
-        <v>4.755818683591979E-18</v>
+        <v>-1.140500250411986E-17</v>
       </c>
       <c r="I43">
-        <v>-8.347727864077691E-19</v>
+        <v>-6.140456163279193E-18</v>
       </c>
       <c r="J43">
-        <v>3.369238156645878E-18</v>
+        <v>-2.759654021669824E-17</v>
       </c>
       <c r="K43">
-        <v>-9.957578707217421E-18</v>
+        <v>-9.465641162042334E-18</v>
       </c>
       <c r="L43">
-        <v>-1.579934326002617E-17</v>
+        <v>-3.48644096404821E-18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed a standard scaler
</commit_message>
<xml_diff>
--- a/tables/monthly_tables/detrended_covar/explained_var_ratio.xlsx
+++ b/tables/monthly_tables/detrended_covar/explained_var_ratio.xlsx
@@ -453,1598 +453,1598 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>0.1338727325201035</v>
+        <v>0.1540466696023941</v>
       </c>
       <c r="B2">
-        <v>0.125913679599762</v>
+        <v>0.1436717659235001</v>
       </c>
       <c r="C2">
-        <v>0.1254069656133652</v>
+        <v>0.1529137194156647</v>
       </c>
       <c r="D2">
-        <v>0.1135641038417816</v>
+        <v>0.1338438987731934</v>
       </c>
       <c r="E2">
-        <v>0.1006886288523674</v>
+        <v>0.1484254449605942</v>
       </c>
       <c r="F2">
-        <v>0.1153330653905869</v>
+        <v>0.1796972900629044</v>
       </c>
       <c r="G2">
-        <v>0.130140632390976</v>
+        <v>0.161013200879097</v>
       </c>
       <c r="H2">
-        <v>0.1135972961783409</v>
+        <v>0.1878795325756073</v>
       </c>
       <c r="I2">
-        <v>0.09922987967729568</v>
+        <v>0.126299574971199</v>
       </c>
       <c r="J2">
-        <v>0.08660564571619034</v>
+        <v>0.1400999575853348</v>
       </c>
       <c r="K2">
-        <v>0.0994059219956398</v>
+        <v>0.1106573268771172</v>
       </c>
       <c r="L2">
-        <v>0.1058914437890053</v>
+        <v>0.1360119134187698</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>0.07261680066585541</v>
+        <v>0.08260048925876617</v>
       </c>
       <c r="B3">
-        <v>0.07883117347955704</v>
+        <v>0.08522038906812668</v>
       </c>
       <c r="C3">
-        <v>0.08991431444883347</v>
+        <v>0.09572503715753555</v>
       </c>
       <c r="D3">
-        <v>0.08436419069766998</v>
+        <v>0.1057999357581139</v>
       </c>
       <c r="E3">
-        <v>0.07691492885351181</v>
+        <v>0.07656228542327881</v>
       </c>
       <c r="F3">
-        <v>0.0730605274438858</v>
+        <v>0.07692169398069382</v>
       </c>
       <c r="G3">
-        <v>0.09675819426774979</v>
+        <v>0.1092979982495308</v>
       </c>
       <c r="H3">
-        <v>0.1048085913062096</v>
+        <v>0.1219117641448975</v>
       </c>
       <c r="I3">
-        <v>0.08888678252696991</v>
+        <v>0.094402976334095</v>
       </c>
       <c r="J3">
-        <v>0.06197302043437958</v>
+        <v>0.06174284219741821</v>
       </c>
       <c r="K3">
-        <v>0.0785071924328804</v>
+        <v>0.08086409419775009</v>
       </c>
       <c r="L3">
-        <v>0.06644423305988312</v>
+        <v>0.07434829324483871</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>0.05996358394622803</v>
+        <v>0.06777635216712952</v>
       </c>
       <c r="B4">
-        <v>0.07267205417156219</v>
+        <v>0.07222197204828262</v>
       </c>
       <c r="C4">
-        <v>0.07124143838882446</v>
+        <v>0.07121098041534424</v>
       </c>
       <c r="D4">
-        <v>0.06932410597801208</v>
+        <v>0.07525238394737244</v>
       </c>
       <c r="E4">
-        <v>0.06020419299602509</v>
+        <v>0.06060677394270897</v>
       </c>
       <c r="F4">
-        <v>0.05449477210640907</v>
+        <v>0.05874933674931526</v>
       </c>
       <c r="G4">
-        <v>0.08448421955108643</v>
+        <v>0.08343839645385742</v>
       </c>
       <c r="H4">
-        <v>0.07690112292766571</v>
+        <v>0.07672960311174393</v>
       </c>
       <c r="I4">
-        <v>0.06306380033493042</v>
+        <v>0.06472543627023697</v>
       </c>
       <c r="J4">
-        <v>0.05895973742008209</v>
+        <v>0.05939293652772903</v>
       </c>
       <c r="K4">
-        <v>0.07013998925685883</v>
+        <v>0.07586430013179779</v>
       </c>
       <c r="L4">
-        <v>0.06244392320513725</v>
+        <v>0.06134888157248497</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>0.05181236192584038</v>
+        <v>0.05377311632037163</v>
       </c>
       <c r="B5">
-        <v>0.05125131085515022</v>
+        <v>0.04885070398449898</v>
       </c>
       <c r="C5">
-        <v>0.05191419646143913</v>
+        <v>0.055483628064394</v>
       </c>
       <c r="D5">
-        <v>0.0520835667848587</v>
+        <v>0.05600150674581528</v>
       </c>
       <c r="E5">
-        <v>0.05191752687096596</v>
+        <v>0.05046369135379791</v>
       </c>
       <c r="F5">
-        <v>0.05335304513573647</v>
+        <v>0.04706563800573349</v>
       </c>
       <c r="G5">
-        <v>0.05007528141140938</v>
+        <v>0.06736797839403152</v>
       </c>
       <c r="H5">
-        <v>0.06451497226953506</v>
+        <v>0.07068275660276413</v>
       </c>
       <c r="I5">
-        <v>0.05422381311655045</v>
+        <v>0.058644849807024</v>
       </c>
       <c r="J5">
-        <v>0.0564587265253067</v>
+        <v>0.05342436209321022</v>
       </c>
       <c r="K5">
-        <v>0.05445414036512375</v>
+        <v>0.06020762398838997</v>
       </c>
       <c r="L5">
-        <v>0.06021403148770332</v>
+        <v>0.05763049051165581</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>0.04734945297241211</v>
+        <v>0.04794770479202271</v>
       </c>
       <c r="B6">
-        <v>0.04718491807579994</v>
+        <v>0.04587119817733765</v>
       </c>
       <c r="C6">
-        <v>0.04352777078747749</v>
+        <v>0.04135908558964729</v>
       </c>
       <c r="D6">
-        <v>0.04469393938779831</v>
+        <v>0.04433756321668625</v>
       </c>
       <c r="E6">
-        <v>0.04704675450921059</v>
+        <v>0.04819374904036522</v>
       </c>
       <c r="F6">
-        <v>0.04945943504571915</v>
+        <v>0.04318183660507202</v>
       </c>
       <c r="G6">
-        <v>0.04439662396907806</v>
+        <v>0.05813895910978317</v>
       </c>
       <c r="H6">
-        <v>0.04725673794746399</v>
+        <v>0.06415216624736786</v>
       </c>
       <c r="I6">
-        <v>0.05093162879347801</v>
+        <v>0.05182994157075882</v>
       </c>
       <c r="J6">
-        <v>0.05174275860190392</v>
+        <v>0.05041475221514702</v>
       </c>
       <c r="K6">
-        <v>0.04552011936903</v>
+        <v>0.04926614090800285</v>
       </c>
       <c r="L6">
-        <v>0.0503842905163765</v>
+        <v>0.05048537999391556</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>0.03926332667469978</v>
+        <v>0.03810396045446396</v>
       </c>
       <c r="B7">
-        <v>0.03933484107255936</v>
+        <v>0.04088213294744492</v>
       </c>
       <c r="C7">
-        <v>0.04087380692362785</v>
+        <v>0.04001501575112343</v>
       </c>
       <c r="D7">
-        <v>0.04106708988547325</v>
+        <v>0.04278664663434029</v>
       </c>
       <c r="E7">
-        <v>0.04564728587865829</v>
+        <v>0.04511215165257454</v>
       </c>
       <c r="F7">
-        <v>0.04507629200816154</v>
+        <v>0.04114799574017525</v>
       </c>
       <c r="G7">
-        <v>0.04034591838717461</v>
+        <v>0.05054560303688049</v>
       </c>
       <c r="H7">
-        <v>0.04318524152040482</v>
+        <v>0.05373971164226532</v>
       </c>
       <c r="I7">
-        <v>0.04617078974843025</v>
+        <v>0.04693720489740372</v>
       </c>
       <c r="J7">
-        <v>0.04378877952694893</v>
+        <v>0.04375197738409042</v>
       </c>
       <c r="K7">
-        <v>0.03884269669651985</v>
+        <v>0.04220477491617203</v>
       </c>
       <c r="L7">
-        <v>0.04242680221796036</v>
+        <v>0.04376854002475739</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>0.0351327657699585</v>
+        <v>0.03494356200098991</v>
       </c>
       <c r="B8">
-        <v>0.03650553897023201</v>
+        <v>0.03681307286024094</v>
       </c>
       <c r="C8">
-        <v>0.03660107403993607</v>
+        <v>0.03700166940689087</v>
       </c>
       <c r="D8">
-        <v>0.03590208664536476</v>
+        <v>0.03666295111179352</v>
       </c>
       <c r="E8">
-        <v>0.03916233405470848</v>
+        <v>0.04039252921938896</v>
       </c>
       <c r="F8">
-        <v>0.03753549233078957</v>
+        <v>0.03713463991880417</v>
       </c>
       <c r="G8">
-        <v>0.03848766908049583</v>
+        <v>0.04226161539554596</v>
       </c>
       <c r="H8">
-        <v>0.03966401144862175</v>
+        <v>0.04149636626243591</v>
       </c>
       <c r="I8">
-        <v>0.0400247797369957</v>
+        <v>0.03791286796331406</v>
       </c>
       <c r="J8">
-        <v>0.03816371038556099</v>
+        <v>0.03802486136555672</v>
       </c>
       <c r="K8">
-        <v>0.03702622279524803</v>
+        <v>0.03600417077541351</v>
       </c>
       <c r="L8">
-        <v>0.03799231350421906</v>
+        <v>0.03732878714799881</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>0.0339016318321228</v>
+        <v>0.03115440905094147</v>
       </c>
       <c r="B9">
-        <v>0.03322781622409821</v>
+        <v>0.03320907801389694</v>
       </c>
       <c r="C9">
-        <v>0.03489253297448158</v>
+        <v>0.03415047749876976</v>
       </c>
       <c r="D9">
-        <v>0.03463001176714897</v>
+        <v>0.0321795642375946</v>
       </c>
       <c r="E9">
-        <v>0.03837613388895988</v>
+        <v>0.0380227230489254</v>
       </c>
       <c r="F9">
-        <v>0.03596978262066841</v>
+        <v>0.034935612231493</v>
       </c>
       <c r="G9">
-        <v>0.03513386845588684</v>
+        <v>0.03464231640100479</v>
       </c>
       <c r="H9">
-        <v>0.03891538083553314</v>
+        <v>0.04065761342644691</v>
       </c>
       <c r="I9">
-        <v>0.03455007448792458</v>
+        <v>0.03463759273290634</v>
       </c>
       <c r="J9">
-        <v>0.03403459489345551</v>
+        <v>0.03357255458831787</v>
       </c>
       <c r="K9">
-        <v>0.03620685264468193</v>
+        <v>0.03411087766289711</v>
       </c>
       <c r="L9">
-        <v>0.03490334376692772</v>
+        <v>0.03475689888000488</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>0.03222085162997246</v>
+        <v>0.0298054926097393</v>
       </c>
       <c r="B10">
-        <v>0.03100530058145523</v>
+        <v>0.0307224728167057</v>
       </c>
       <c r="C10">
-        <v>0.03237501531839371</v>
+        <v>0.03075847774744034</v>
       </c>
       <c r="D10">
-        <v>0.032764732837677</v>
+        <v>0.029708631336689</v>
       </c>
       <c r="E10">
-        <v>0.03147232159972191</v>
+        <v>0.03099767863750458</v>
       </c>
       <c r="F10">
-        <v>0.03404843807220459</v>
+        <v>0.03261736035346985</v>
       </c>
       <c r="G10">
-        <v>0.03183456137776375</v>
+        <v>0.03396565467119217</v>
       </c>
       <c r="H10">
-        <v>0.03400585427880287</v>
+        <v>0.03423395380377769</v>
       </c>
       <c r="I10">
-        <v>0.03240593150258064</v>
+        <v>0.03382493555545807</v>
       </c>
       <c r="J10">
-        <v>0.03331540897488594</v>
+        <v>0.03168575465679169</v>
       </c>
       <c r="K10">
-        <v>0.03267784789204597</v>
+        <v>0.03337752446532249</v>
       </c>
       <c r="L10">
-        <v>0.03160518407821655</v>
+        <v>0.03127147257328033</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>0.02706059440970421</v>
+        <v>0.02725474908947945</v>
       </c>
       <c r="B11">
-        <v>0.02918297052383423</v>
+        <v>0.02864658832550049</v>
       </c>
       <c r="C11">
-        <v>0.03002505004405975</v>
+        <v>0.02811707183718681</v>
       </c>
       <c r="D11">
-        <v>0.02894779667258263</v>
+        <v>0.02843679115176201</v>
       </c>
       <c r="E11">
-        <v>0.0306889358907938</v>
+        <v>0.02767338044941425</v>
       </c>
       <c r="F11">
-        <v>0.03169231116771698</v>
+        <v>0.02977876923978329</v>
       </c>
       <c r="G11">
-        <v>0.02915521711111069</v>
+        <v>0.029640793800354</v>
       </c>
       <c r="H11">
-        <v>0.03169717267155647</v>
+        <v>0.03129624575376511</v>
       </c>
       <c r="I11">
-        <v>0.02926719188690186</v>
+        <v>0.02765061892569065</v>
       </c>
       <c r="J11">
-        <v>0.03150303289294243</v>
+        <v>0.03100094571709633</v>
       </c>
       <c r="K11">
-        <v>0.03036756068468094</v>
+        <v>0.02945965528488159</v>
       </c>
       <c r="L11">
-        <v>0.0302783977240324</v>
+        <v>0.02959606423974037</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>0.02686254866421223</v>
+        <v>0.02604818902909756</v>
       </c>
       <c r="B12">
-        <v>0.02587605081498623</v>
+        <v>0.02622147090733051</v>
       </c>
       <c r="C12">
-        <v>0.02667060494422913</v>
+        <v>0.02554437331855297</v>
       </c>
       <c r="D12">
-        <v>0.02739734388887882</v>
+        <v>0.02670996077358723</v>
       </c>
       <c r="E12">
-        <v>0.02735623717308044</v>
+        <v>0.02603122778236866</v>
       </c>
       <c r="F12">
-        <v>0.02984047308564186</v>
+        <v>0.02903450839221478</v>
       </c>
       <c r="G12">
-        <v>0.02799607627093792</v>
+        <v>0.02769465930759907</v>
       </c>
       <c r="H12">
-        <v>0.03028761595487595</v>
+        <v>0.02701626531779766</v>
       </c>
       <c r="I12">
-        <v>0.02681435830891132</v>
+        <v>0.02667217887938023</v>
       </c>
       <c r="J12">
-        <v>0.02997447736561298</v>
+        <v>0.02831370756030083</v>
       </c>
       <c r="K12">
-        <v>0.02924154512584209</v>
+        <v>0.02706044912338257</v>
       </c>
       <c r="L12">
-        <v>0.02802326716482639</v>
+        <v>0.02641757763922215</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>0.02552771754562855</v>
+        <v>0.02292131818830967</v>
       </c>
       <c r="B13">
-        <v>0.02554875239729881</v>
+        <v>0.02440133318305016</v>
       </c>
       <c r="C13">
-        <v>0.02532735094428062</v>
+        <v>0.02439648844301701</v>
       </c>
       <c r="D13">
-        <v>0.02631004899740219</v>
+        <v>0.02345546893775463</v>
       </c>
       <c r="E13">
-        <v>0.02497809194028378</v>
+        <v>0.02405558153986931</v>
       </c>
       <c r="F13">
-        <v>0.02740764617919922</v>
+        <v>0.02646380104124546</v>
       </c>
       <c r="G13">
-        <v>0.02491389587521553</v>
+        <v>0.02607322111725807</v>
       </c>
       <c r="H13">
-        <v>0.02651687152683735</v>
+        <v>0.02542679943144321</v>
       </c>
       <c r="I13">
-        <v>0.02580179646611214</v>
+        <v>0.0245075449347496</v>
       </c>
       <c r="J13">
-        <v>0.02679777331650257</v>
+        <v>0.02537010423839092</v>
       </c>
       <c r="K13">
-        <v>0.02786619588732719</v>
+        <v>0.02529070526361465</v>
       </c>
       <c r="L13">
-        <v>0.02674411423504353</v>
+        <v>0.02530816942453384</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>0.0235342625528574</v>
+        <v>0.02246272563934326</v>
       </c>
       <c r="B14">
-        <v>0.02301761135458946</v>
+        <v>0.02388767153024673</v>
       </c>
       <c r="C14">
-        <v>0.02359144017100334</v>
+        <v>0.02259504795074463</v>
       </c>
       <c r="D14">
-        <v>0.02326559834182262</v>
+        <v>0.02232108265161514</v>
       </c>
       <c r="E14">
-        <v>0.02480421774089336</v>
+        <v>0.02345040254294872</v>
       </c>
       <c r="F14">
-        <v>0.02571313641965389</v>
+        <v>0.02442043274641037</v>
       </c>
       <c r="G14">
-        <v>0.02446543239057064</v>
+        <v>0.02532447688281536</v>
       </c>
       <c r="H14">
-        <v>0.02498333714902401</v>
+        <v>0.02246112003922462</v>
       </c>
       <c r="I14">
-        <v>0.02465181052684784</v>
+        <v>0.02406102977693081</v>
       </c>
       <c r="J14">
-        <v>0.02530659735202789</v>
+        <v>0.02442105486989021</v>
       </c>
       <c r="K14">
-        <v>0.02553184516727924</v>
+        <v>0.02398838475346565</v>
       </c>
       <c r="L14">
-        <v>0.02602857910096645</v>
+        <v>0.02434155344963074</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>0.02311912178993225</v>
+        <v>0.0219894964247942</v>
       </c>
       <c r="B15">
-        <v>0.02214928530156612</v>
+        <v>0.02212552353739738</v>
       </c>
       <c r="C15">
-        <v>0.02284772321581841</v>
+        <v>0.02094489522278309</v>
       </c>
       <c r="D15">
-        <v>0.02300520054996014</v>
+        <v>0.02092092484235764</v>
       </c>
       <c r="E15">
-        <v>0.02390498109161854</v>
+        <v>0.02310598827898502</v>
       </c>
       <c r="F15">
-        <v>0.02438764460384846</v>
+        <v>0.02431748807430267</v>
       </c>
       <c r="G15">
-        <v>0.02369608543813229</v>
+        <v>0.02287687547504902</v>
       </c>
       <c r="H15">
-        <v>0.0245379377156496</v>
+        <v>0.01952852122485638</v>
       </c>
       <c r="I15">
-        <v>0.02344422228634357</v>
+        <v>0.02382857166230679</v>
       </c>
       <c r="J15">
-        <v>0.02483338862657547</v>
+        <v>0.02300246618688107</v>
       </c>
       <c r="K15">
-        <v>0.02338248863816261</v>
+        <v>0.0237241480499506</v>
       </c>
       <c r="L15">
-        <v>0.0234102476388216</v>
+        <v>0.02329171635210514</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>0.0227822121232748</v>
+        <v>0.02094465866684914</v>
       </c>
       <c r="B16">
-        <v>0.02153196558356285</v>
+        <v>0.02094953693449497</v>
       </c>
       <c r="C16">
-        <v>0.02136997319757938</v>
+        <v>0.0199552308768034</v>
       </c>
       <c r="D16">
-        <v>0.02076604589819908</v>
+        <v>0.01929977349936962</v>
       </c>
       <c r="E16">
-        <v>0.02191208861768246</v>
+        <v>0.02170292474329472</v>
       </c>
       <c r="F16">
-        <v>0.02283885143697262</v>
+        <v>0.02248851023614407</v>
       </c>
       <c r="G16">
-        <v>0.02186628989875317</v>
+        <v>0.02007030509412289</v>
       </c>
       <c r="H16">
-        <v>0.0218051802366972</v>
+        <v>0.01866349391639233</v>
       </c>
       <c r="I16">
-        <v>0.02186517231166363</v>
+        <v>0.02211959660053253</v>
       </c>
       <c r="J16">
-        <v>0.02340684272348881</v>
+        <v>0.02227050997316837</v>
       </c>
       <c r="K16">
-        <v>0.0213842149823904</v>
+        <v>0.02141766808927059</v>
       </c>
       <c r="L16">
-        <v>0.02274024672806263</v>
+        <v>0.02197401784360409</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>0.02197181433439255</v>
+        <v>0.02063743025064468</v>
       </c>
       <c r="B17">
-        <v>0.02081560529768467</v>
+        <v>0.0201976727694273</v>
       </c>
       <c r="C17">
-        <v>0.01956178434193134</v>
+        <v>0.0191799458116293</v>
       </c>
       <c r="D17">
-        <v>0.02022920735180378</v>
+        <v>0.01886372640728951</v>
       </c>
       <c r="E17">
-        <v>0.02141768857836723</v>
+        <v>0.02101371996104717</v>
       </c>
       <c r="F17">
-        <v>0.02210044860839844</v>
+        <v>0.02072435058653355</v>
       </c>
       <c r="G17">
-        <v>0.02091233618557453</v>
+        <v>0.01919856294989586</v>
       </c>
       <c r="H17">
-        <v>0.02170257829129696</v>
+        <v>0.0161858331412077</v>
       </c>
       <c r="I17">
-        <v>0.02101203054189682</v>
+        <v>0.0205991230905056</v>
       </c>
       <c r="J17">
-        <v>0.02315941825509071</v>
+        <v>0.02172798104584217</v>
       </c>
       <c r="K17">
-        <v>0.02074450999498367</v>
+        <v>0.0209356676787138</v>
       </c>
       <c r="L17">
-        <v>0.02158032916486263</v>
+        <v>0.02144632302224636</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>0.02059073001146317</v>
+        <v>0.01986415311694145</v>
       </c>
       <c r="B18">
-        <v>0.02009419724345207</v>
+        <v>0.01803815923631191</v>
       </c>
       <c r="C18">
-        <v>0.01939327456057072</v>
+        <v>0.01878634095191956</v>
       </c>
       <c r="D18">
-        <v>0.01957697235047817</v>
+        <v>0.01772851496934891</v>
       </c>
       <c r="E18">
-        <v>0.02051487006247044</v>
+        <v>0.0192185714840889</v>
       </c>
       <c r="F18">
-        <v>0.02189897559583187</v>
+        <v>0.01971588656306267</v>
       </c>
       <c r="G18">
-        <v>0.01971432566642761</v>
+        <v>0.01743770390748978</v>
       </c>
       <c r="H18">
-        <v>0.01914337649941444</v>
+        <v>0.01517961360514164</v>
       </c>
       <c r="I18">
-        <v>0.02035017684102058</v>
+        <v>0.01979006454348564</v>
       </c>
       <c r="J18">
-        <v>0.02133136801421642</v>
+        <v>0.02013545110821724</v>
       </c>
       <c r="K18">
-        <v>0.01987983286380768</v>
+        <v>0.01901177689433098</v>
       </c>
       <c r="L18">
-        <v>0.02030050568282604</v>
+        <v>0.01894095540046692</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>0.02013366483151913</v>
+        <v>0.01832872070372105</v>
       </c>
       <c r="B19">
-        <v>0.01791338808834553</v>
+        <v>0.01761769689619541</v>
       </c>
       <c r="C19">
-        <v>0.01820914074778557</v>
+        <v>0.01712684705853462</v>
       </c>
       <c r="D19">
-        <v>0.01905861124396324</v>
+        <v>0.01669115573167801</v>
       </c>
       <c r="E19">
-        <v>0.01994836516678333</v>
+        <v>0.01841823942959309</v>
       </c>
       <c r="F19">
-        <v>0.02083017490804195</v>
+        <v>0.01905820704996586</v>
       </c>
       <c r="G19">
-        <v>0.01911592297255993</v>
+        <v>0.01675940118730068</v>
       </c>
       <c r="H19">
-        <v>0.01818354055285454</v>
+        <v>0.01418541837483644</v>
       </c>
       <c r="I19">
-        <v>0.01939662359654903</v>
+        <v>0.01811493560671806</v>
       </c>
       <c r="J19">
-        <v>0.02112765423953533</v>
+        <v>0.01992383599281311</v>
       </c>
       <c r="K19">
-        <v>0.0195916797965765</v>
+        <v>0.0183428842574358</v>
       </c>
       <c r="L19">
-        <v>0.01990029588341713</v>
+        <v>0.01823623850941658</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>0.01849491335451603</v>
+        <v>0.01717695407569408</v>
       </c>
       <c r="B20">
-        <v>0.01766425371170044</v>
+        <v>0.01727506518363953</v>
       </c>
       <c r="C20">
-        <v>0.01802777498960495</v>
+        <v>0.01666493900120258</v>
       </c>
       <c r="D20">
-        <v>0.01871654950082302</v>
+        <v>0.01661882176995277</v>
       </c>
       <c r="E20">
-        <v>0.01893363893032074</v>
+        <v>0.0174632091075182</v>
       </c>
       <c r="F20">
-        <v>0.01932000182569027</v>
+        <v>0.01850658655166626</v>
       </c>
       <c r="G20">
-        <v>0.01721378043293953</v>
+        <v>0.01583448797464371</v>
       </c>
       <c r="H20">
-        <v>0.01792038045823574</v>
+        <v>0.01271967962384224</v>
       </c>
       <c r="I20">
-        <v>0.01875429227948189</v>
+        <v>0.01739084161818027</v>
       </c>
       <c r="J20">
-        <v>0.02049494348466396</v>
+        <v>0.01854800991714001</v>
       </c>
       <c r="K20">
-        <v>0.01899986527860165</v>
+        <v>0.01784904487431049</v>
       </c>
       <c r="L20">
-        <v>0.0184646975249052</v>
+        <v>0.01757879182696342</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>0.01806804724037647</v>
+        <v>0.01670820824801922</v>
       </c>
       <c r="B21">
-        <v>0.01679598540067673</v>
+        <v>0.01657586172223091</v>
       </c>
       <c r="C21">
-        <v>0.0165567509829998</v>
+        <v>0.0163764450699091</v>
       </c>
       <c r="D21">
-        <v>0.01811051368713379</v>
+        <v>0.01583220809698105</v>
       </c>
       <c r="E21">
-        <v>0.01849042437970638</v>
+        <v>0.0164004061371088</v>
       </c>
       <c r="F21">
-        <v>0.01833630912005901</v>
+        <v>0.01686098799109459</v>
       </c>
       <c r="G21">
-        <v>0.01670115627348423</v>
+        <v>0.01553476415574551</v>
       </c>
       <c r="H21">
-        <v>0.01706064864993095</v>
+        <v>0.01178583037108183</v>
       </c>
       <c r="I21">
-        <v>0.01790322735905647</v>
+        <v>0.01640698499977589</v>
       </c>
       <c r="J21">
-        <v>0.01950682327151299</v>
+        <v>0.01728167943656445</v>
       </c>
       <c r="K21">
-        <v>0.0181496050208807</v>
+        <v>0.01704102382063866</v>
       </c>
       <c r="L21">
-        <v>0.01805507205426693</v>
+        <v>0.01659355312585831</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22">
-        <v>0.01781157776713371</v>
+        <v>0.01598734222352505</v>
       </c>
       <c r="B22">
-        <v>0.01647081971168518</v>
+        <v>0.01572113484144211</v>
       </c>
       <c r="C22">
-        <v>0.01630770228803158</v>
+        <v>0.01527933776378632</v>
       </c>
       <c r="D22">
-        <v>0.01747447438538074</v>
+        <v>0.01519269589334726</v>
       </c>
       <c r="E22">
-        <v>0.01749840565025806</v>
+        <v>0.01593601517379284</v>
       </c>
       <c r="F22">
-        <v>0.01724046841263771</v>
+        <v>0.01646662876009941</v>
       </c>
       <c r="G22">
-        <v>0.01651702076196671</v>
+        <v>0.01352704968303442</v>
       </c>
       <c r="H22">
-        <v>0.01541793160140514</v>
+        <v>0.01086101494729519</v>
       </c>
       <c r="I22">
-        <v>0.01721618324518204</v>
+        <v>0.0163402296602726</v>
       </c>
       <c r="J22">
-        <v>0.01853544823825359</v>
+        <v>0.01696905866265297</v>
       </c>
       <c r="K22">
-        <v>0.01736951805651188</v>
+        <v>0.01670266874134541</v>
       </c>
       <c r="L22">
-        <v>0.0174203235656023</v>
+        <v>0.01635354943573475</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23">
-        <v>0.01693591848015785</v>
+        <v>0.01534860301762819</v>
       </c>
       <c r="B23">
-        <v>0.01631209440529346</v>
+        <v>0.01538108196109533</v>
       </c>
       <c r="C23">
-        <v>0.0157068595290184</v>
+        <v>0.01457453984767199</v>
       </c>
       <c r="D23">
-        <v>0.0169783029705286</v>
+        <v>0.01501145213842392</v>
       </c>
       <c r="E23">
-        <v>0.01742576994001865</v>
+        <v>0.01551701594144106</v>
       </c>
       <c r="F23">
-        <v>0.01675828918814659</v>
+        <v>0.01528436876833439</v>
       </c>
       <c r="G23">
-        <v>0.01553167682141066</v>
+        <v>0.01250700280070305</v>
       </c>
       <c r="H23">
-        <v>0.01460942905396223</v>
+        <v>0.010362533852458</v>
       </c>
       <c r="I23">
-        <v>0.0165436640381813</v>
+        <v>0.01595100574195385</v>
       </c>
       <c r="J23">
-        <v>0.01777249947190285</v>
+        <v>0.0158030204474926</v>
       </c>
       <c r="K23">
-        <v>0.01699396036565304</v>
+        <v>0.01614733412861824</v>
       </c>
       <c r="L23">
-        <v>0.01664020493626595</v>
+        <v>0.01528040319681168</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24">
-        <v>0.01594242267310619</v>
+        <v>0.01460514031350613</v>
       </c>
       <c r="B24">
-        <v>0.01599110476672649</v>
+        <v>0.01460400503128767</v>
       </c>
       <c r="C24">
-        <v>0.01530432235449553</v>
+        <v>0.01412987429648638</v>
       </c>
       <c r="D24">
-        <v>0.01618009619414806</v>
+        <v>0.01405080873519182</v>
       </c>
       <c r="E24">
-        <v>0.01647685654461384</v>
+        <v>0.01472212374210358</v>
       </c>
       <c r="F24">
-        <v>0.01655388996005058</v>
+        <v>0.01431984640657902</v>
       </c>
       <c r="G24">
-        <v>0.01528688706457615</v>
+        <v>0.01167355012148619</v>
       </c>
       <c r="H24">
-        <v>0.01406727358698845</v>
+        <v>0.009247911162674427</v>
       </c>
       <c r="I24">
-        <v>0.01553751900792122</v>
+        <v>0.0142455268651247</v>
       </c>
       <c r="J24">
-        <v>0.01652782782912254</v>
+        <v>0.01526676770299673</v>
       </c>
       <c r="K24">
-        <v>0.0162002369761467</v>
+        <v>0.01582770608365536</v>
       </c>
       <c r="L24">
-        <v>0.01579614169895649</v>
+        <v>0.01501198206096888</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25">
-        <v>0.01521469838917255</v>
+        <v>0.01419590879231691</v>
       </c>
       <c r="B25">
-        <v>0.01523143518716097</v>
+        <v>0.01400429848581553</v>
       </c>
       <c r="C25">
-        <v>0.01528398599475622</v>
+        <v>0.01314501836895943</v>
       </c>
       <c r="D25">
-        <v>0.01552731916308403</v>
+        <v>0.01346247084438801</v>
       </c>
       <c r="E25">
-        <v>0.01588810794055462</v>
+        <v>0.01405343133956194</v>
       </c>
       <c r="F25">
-        <v>0.01547235809266567</v>
+        <v>0.01372593455016613</v>
       </c>
       <c r="G25">
-        <v>0.01463638059794903</v>
+        <v>0.01070098578929901</v>
       </c>
       <c r="H25">
-        <v>0.01355749368667603</v>
+        <v>0.00803010817617178</v>
       </c>
       <c r="I25">
-        <v>0.01526197791099548</v>
+        <v>0.01389339007437229</v>
       </c>
       <c r="J25">
-        <v>0.01624478399753571</v>
+        <v>0.01487740874290466</v>
       </c>
       <c r="K25">
-        <v>0.01595295965671539</v>
+        <v>0.01532264426350594</v>
       </c>
       <c r="L25">
-        <v>0.01535311713814735</v>
+        <v>0.01397649943828583</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26">
-        <v>0.014626226387918</v>
+        <v>0.01350014936178923</v>
       </c>
       <c r="B26">
-        <v>0.01483239699155092</v>
+        <v>0.01344877015799284</v>
       </c>
       <c r="C26">
-        <v>0.01442141178995371</v>
+        <v>0.01303613092750311</v>
       </c>
       <c r="D26">
-        <v>0.01497383788228035</v>
+        <v>0.0128914276137948</v>
       </c>
       <c r="E26">
-        <v>0.01534202136099339</v>
+        <v>0.01373191922903061</v>
       </c>
       <c r="F26">
-        <v>0.01473985053598881</v>
+        <v>0.0132618797942996</v>
       </c>
       <c r="G26">
-        <v>0.01383868977427483</v>
+        <v>0.01001567114144564</v>
       </c>
       <c r="H26">
-        <v>0.01207165978848934</v>
+        <v>0.007929501123726368</v>
       </c>
       <c r="I26">
-        <v>0.01457644067704678</v>
+        <v>0.01324925851076841</v>
       </c>
       <c r="J26">
-        <v>0.01565666124224663</v>
+        <v>0.01448987144976854</v>
       </c>
       <c r="K26">
-        <v>0.01564572378993034</v>
+        <v>0.01381462253630161</v>
       </c>
       <c r="L26">
-        <v>0.01505765784531832</v>
+        <v>0.01374496147036552</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27">
-        <v>0.01419575046747923</v>
+        <v>0.01340894866734743</v>
       </c>
       <c r="B27">
-        <v>0.01358369924128056</v>
+        <v>0.01321818772703409</v>
       </c>
       <c r="C27">
-        <v>0.01306109596043825</v>
+        <v>0.01241404376924038</v>
       </c>
       <c r="D27">
-        <v>0.01443131919950247</v>
+        <v>0.0125120161101222</v>
       </c>
       <c r="E27">
-        <v>0.01520273182541132</v>
+        <v>0.01359198242425919</v>
       </c>
       <c r="F27">
-        <v>0.01351428963243961</v>
+        <v>0.0124530466273427</v>
       </c>
       <c r="G27">
-        <v>0.01247220486402512</v>
+        <v>0.00937363225966692</v>
       </c>
       <c r="H27">
-        <v>0.01145222596824169</v>
+        <v>0.007029804401099682</v>
       </c>
       <c r="I27">
-        <v>0.01418257225304842</v>
+        <v>0.0127192260697484</v>
       </c>
       <c r="J27">
-        <v>0.01528591476380825</v>
+        <v>0.01409793831408024</v>
       </c>
       <c r="K27">
-        <v>0.0147757101804018</v>
+        <v>0.01357180159538984</v>
       </c>
       <c r="L27">
-        <v>0.01465476863086224</v>
+        <v>0.01350407395511866</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28">
-        <v>0.013718631118536</v>
+        <v>0.01256871316581964</v>
       </c>
       <c r="B28">
-        <v>0.01344456151127815</v>
+        <v>0.01265309937298298</v>
       </c>
       <c r="C28">
-        <v>0.0125372689217329</v>
+        <v>0.01223320234566927</v>
       </c>
       <c r="D28">
-        <v>0.01409287378191948</v>
+        <v>0.01230170764029026</v>
       </c>
       <c r="E28">
-        <v>0.01470145490020514</v>
+        <v>0.01273084059357643</v>
       </c>
       <c r="F28">
-        <v>0.01320374384522438</v>
+        <v>0.01194181572645903</v>
       </c>
       <c r="G28">
-        <v>0.01198144350200891</v>
+        <v>0.008825378492474556</v>
       </c>
       <c r="H28">
-        <v>0.01126179657876492</v>
+        <v>0.00538953859359026</v>
       </c>
       <c r="I28">
-        <v>0.01408970262855291</v>
+        <v>0.01243997924029827</v>
       </c>
       <c r="J28">
-        <v>0.01478192117065191</v>
+        <v>0.01344418060034513</v>
       </c>
       <c r="K28">
-        <v>0.01411791518330574</v>
+        <v>0.01316928677260876</v>
       </c>
       <c r="L28">
-        <v>0.01442981604486704</v>
+        <v>0.01251043565571308</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29">
-        <v>0.01310729887336493</v>
+        <v>0.01185538060963154</v>
       </c>
       <c r="B29">
-        <v>0.01311674062162638</v>
+        <v>0.01206330675631762</v>
       </c>
       <c r="C29">
-        <v>0.01230484433472157</v>
+        <v>0.01107888296246529</v>
       </c>
       <c r="D29">
-        <v>0.01358349155634642</v>
+        <v>0.01208884082734585</v>
       </c>
       <c r="E29">
-        <v>0.01418054290115833</v>
+        <v>0.01255736406892538</v>
       </c>
       <c r="F29">
-        <v>0.01262332499027252</v>
+        <v>0.01127763465046883</v>
       </c>
       <c r="G29">
-        <v>0.01130457129329443</v>
+        <v>0.007844523526728153</v>
       </c>
       <c r="H29">
-        <v>0.01071085594594479</v>
+        <v>0.005043220240622759</v>
       </c>
       <c r="I29">
-        <v>0.01319137308746576</v>
+        <v>0.01208919379860163</v>
       </c>
       <c r="J29">
-        <v>0.01439712475985289</v>
+        <v>0.01330140326172113</v>
       </c>
       <c r="K29">
-        <v>0.01379486359655857</v>
+        <v>0.0130154974758625</v>
       </c>
       <c r="L29">
-        <v>0.01334571279585361</v>
+        <v>0.01204364746809006</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30">
-        <v>0.01292108837515116</v>
+        <v>0.01173421833664179</v>
       </c>
       <c r="B30">
-        <v>0.01261907257139683</v>
+        <v>0.01199247688055038</v>
       </c>
       <c r="C30">
-        <v>0.01161875762045383</v>
+        <v>0.01051468495279551</v>
       </c>
       <c r="D30">
-        <v>0.01267289556562901</v>
+        <v>0.01106126699596643</v>
       </c>
       <c r="E30">
-        <v>0.01331024710088968</v>
+        <v>0.0110156936571002</v>
       </c>
       <c r="F30">
-        <v>0.01214020140469074</v>
+        <v>0.0105032054707408</v>
       </c>
       <c r="G30">
-        <v>0.01071824878454208</v>
+        <v>0.007164183538407087</v>
       </c>
       <c r="H30">
-        <v>0.01035148277878761</v>
+        <v>0.00499492883682251</v>
       </c>
       <c r="I30">
-        <v>0.01284029427915812</v>
+        <v>0.01121056266129017</v>
       </c>
       <c r="J30">
-        <v>0.01427466794848442</v>
+        <v>0.01279523130506277</v>
       </c>
       <c r="K30">
-        <v>0.0130575904622674</v>
+        <v>0.01229647174477577</v>
       </c>
       <c r="L30">
-        <v>0.01296994090080261</v>
+        <v>0.01182152982801199</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31">
-        <v>0.0123857157304883</v>
+        <v>0.01135226059705019</v>
       </c>
       <c r="B31">
-        <v>0.01227681897580624</v>
+        <v>0.01139667816460133</v>
       </c>
       <c r="C31">
-        <v>0.01150182168930769</v>
+        <v>0.01048269867897034</v>
       </c>
       <c r="D31">
-        <v>0.01254683639854193</v>
+        <v>0.01105167344212532</v>
       </c>
       <c r="E31">
-        <v>0.01262989733368158</v>
+        <v>0.01092521566897631</v>
       </c>
       <c r="F31">
-        <v>0.01169313117861748</v>
+        <v>0.009907309897243977</v>
       </c>
       <c r="G31">
-        <v>0.01030728127807379</v>
+        <v>0.005231616552919149</v>
       </c>
       <c r="H31">
-        <v>0.00905653927475214</v>
+        <v>0.004385207779705524</v>
       </c>
       <c r="I31">
-        <v>0.01246047671884298</v>
+        <v>0.01067816559225321</v>
       </c>
       <c r="J31">
-        <v>0.01405965443700552</v>
+        <v>0.01153209619224072</v>
       </c>
       <c r="K31">
-        <v>0.01263730227947235</v>
+        <v>0.01162285730242729</v>
       </c>
       <c r="L31">
-        <v>0.01241208240389824</v>
+        <v>0.0113725708797574</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32">
-        <v>0.01213699579238892</v>
+        <v>0.0111070666462183</v>
       </c>
       <c r="B32">
-        <v>0.01185929961502552</v>
+        <v>0.01075896993279457</v>
       </c>
       <c r="C32">
-        <v>0.01111058704555035</v>
+        <v>0.0100791035220027</v>
       </c>
       <c r="D32">
-        <v>0.01161486189812422</v>
+        <v>0.01066647469997406</v>
       </c>
       <c r="E32">
-        <v>0.0122300498187542</v>
+        <v>0.01036423724144697</v>
       </c>
       <c r="F32">
-        <v>0.01143319997936487</v>
+        <v>0.009590565226972103</v>
       </c>
       <c r="G32">
-        <v>0.009905739687383175</v>
+        <v>0.005008658859878778</v>
       </c>
       <c r="H32">
-        <v>0.008501225151121616</v>
+        <v>0.003483149223029613</v>
       </c>
       <c r="I32">
-        <v>0.01205092389136553</v>
+        <v>0.01012669317424297</v>
       </c>
       <c r="J32">
-        <v>0.0131826139986515</v>
+        <v>0.0113270990550518</v>
       </c>
       <c r="K32">
-        <v>0.01226294133812189</v>
+        <v>0.01119515206664801</v>
       </c>
       <c r="L32">
-        <v>0.01222090143710375</v>
+        <v>0.01111603900790215</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33">
-        <v>0.01162144169211388</v>
+        <v>0.01043945364654064</v>
       </c>
       <c r="B33">
-        <v>0.01180180441588163</v>
+        <v>0.01048992481082678</v>
       </c>
       <c r="C33">
-        <v>0.01090835314244032</v>
+        <v>0.009718542918562889</v>
       </c>
       <c r="D33">
-        <v>0.01125151757150888</v>
+        <v>0.01004316471517086</v>
       </c>
       <c r="E33">
-        <v>0.01150191482156515</v>
+        <v>0.01027740817517042</v>
       </c>
       <c r="F33">
-        <v>0.01104834489524364</v>
+        <v>0.008203228935599327</v>
       </c>
       <c r="G33">
-        <v>0.009626044891774654</v>
+        <v>0.004219481721520424</v>
       </c>
       <c r="H33">
-        <v>0.008199214935302734</v>
+        <v>0.003195461118593812</v>
       </c>
       <c r="I33">
-        <v>0.01161912176758051</v>
+        <v>0.009920042939484119</v>
       </c>
       <c r="J33">
-        <v>0.01261330582201481</v>
+        <v>0.01074748858809471</v>
       </c>
       <c r="K33">
-        <v>0.01174215413630009</v>
+        <v>0.01063786260783672</v>
       </c>
       <c r="L33">
-        <v>0.01191827561706305</v>
+        <v>0.01072356477379799</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>0.01131583284586668</v>
+        <v>0.01003080978989601</v>
       </c>
       <c r="B34">
-        <v>0.01135042309761047</v>
+        <v>0.01027902588248253</v>
       </c>
       <c r="C34">
-        <v>0.01084571331739426</v>
+        <v>0.009473014622926712</v>
       </c>
       <c r="D34">
-        <v>0.01068673748522997</v>
+        <v>0.009552170522511005</v>
       </c>
       <c r="E34">
-        <v>0.01139800436794758</v>
+        <v>0.01014296431094408</v>
       </c>
       <c r="F34">
-        <v>0.01038925722241402</v>
+        <v>0.008129715919494629</v>
       </c>
       <c r="G34">
-        <v>0.00877098273485899</v>
+        <v>0.003694287734106183</v>
       </c>
       <c r="H34">
-        <v>0.007357378955930471</v>
+        <v>0.003019984578713775</v>
       </c>
       <c r="I34">
-        <v>0.01105201058089733</v>
+        <v>0.009444658644497395</v>
       </c>
       <c r="J34">
-        <v>0.01206321083009243</v>
+        <v>0.01029715873301029</v>
       </c>
       <c r="K34">
-        <v>0.01117938663810492</v>
+        <v>0.01016859617084265</v>
       </c>
       <c r="L34">
-        <v>0.01150178164243698</v>
+        <v>0.01036552246659994</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35">
-        <v>0.0104821128770709</v>
+        <v>0.009574299678206444</v>
       </c>
       <c r="B35">
-        <v>0.01074813678860664</v>
+        <v>0.01004731189459562</v>
       </c>
       <c r="C35">
-        <v>0.009899848140776157</v>
+        <v>0.009242396801710129</v>
       </c>
       <c r="D35">
-        <v>0.01044658478349447</v>
+        <v>0.00906362384557724</v>
       </c>
       <c r="E35">
-        <v>0.01108317635953426</v>
+        <v>0.009645615704357624</v>
       </c>
       <c r="F35">
-        <v>0.01005436852574348</v>
+        <v>0.007753146346658468</v>
       </c>
       <c r="G35">
-        <v>0.008319420740008354</v>
+        <v>0.003496302058920264</v>
       </c>
       <c r="H35">
-        <v>0.006997388321906328</v>
+        <v>0.002255168743431568</v>
       </c>
       <c r="I35">
-        <v>0.01037596724927425</v>
+        <v>0.008799300529062748</v>
       </c>
       <c r="J35">
-        <v>0.01161073241382837</v>
+        <v>0.009918451309204102</v>
       </c>
       <c r="K35">
-        <v>0.01071303896605968</v>
+        <v>0.009577101096510887</v>
       </c>
       <c r="L35">
-        <v>0.01105089019984007</v>
+        <v>0.01002537086606026</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>0.009944981895387173</v>
+        <v>0.009277171455323696</v>
       </c>
       <c r="B36">
-        <v>0.01029569189995527</v>
+        <v>0.009598621167242527</v>
       </c>
       <c r="C36">
-        <v>0.00941824447363615</v>
+        <v>0.008547507226467133</v>
       </c>
       <c r="D36">
-        <v>0.01018671318888664</v>
+        <v>0.008900885470211506</v>
       </c>
       <c r="E36">
-        <v>0.01076070219278336</v>
+        <v>0.009157950058579445</v>
       </c>
       <c r="F36">
-        <v>0.009745310060679913</v>
+        <v>0.007237490732222795</v>
       </c>
       <c r="G36">
-        <v>0.008252592757344246</v>
+        <v>0.002927323104813695</v>
       </c>
       <c r="H36">
-        <v>0.00611509196460247</v>
+        <v>0.002045462606474757</v>
       </c>
       <c r="I36">
-        <v>0.01019783411175013</v>
+        <v>0.008441600017249584</v>
       </c>
       <c r="J36">
-        <v>0.011118502356112</v>
+        <v>0.009634651243686676</v>
       </c>
       <c r="K36">
-        <v>0.01066502928733826</v>
+        <v>0.009100019000470638</v>
       </c>
       <c r="L36">
-        <v>0.01077342312783003</v>
+        <v>0.009660553187131882</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37">
-        <v>0.009422116912901402</v>
+        <v>0.009061198681592941</v>
       </c>
       <c r="B37">
-        <v>0.009532776661217213</v>
+        <v>0.008672243915498257</v>
       </c>
       <c r="C37">
-        <v>0.00900116004049778</v>
+        <v>0.008194832131266594</v>
       </c>
       <c r="D37">
-        <v>0.009436988271772861</v>
+        <v>0.008380995132029057</v>
       </c>
       <c r="E37">
-        <v>0.01012436114251614</v>
+        <v>0.008556809276342392</v>
       </c>
       <c r="F37">
-        <v>0.009606944397091866</v>
+        <v>0.006602155044674873</v>
       </c>
       <c r="G37">
-        <v>0.006952146999537945</v>
+        <v>0.002507664728909731</v>
       </c>
       <c r="H37">
-        <v>0.005888469982892275</v>
+        <v>0.001795503194443882</v>
       </c>
       <c r="I37">
-        <v>0.009070970118045807</v>
+        <v>0.007439527194947004</v>
       </c>
       <c r="J37">
-        <v>0.01064382772892714</v>
+        <v>0.009305441752076149</v>
       </c>
       <c r="K37">
-        <v>0.0100942263379693</v>
+        <v>0.0089308125898242</v>
       </c>
       <c r="L37">
-        <v>0.0103760277852416</v>
+        <v>0.009284342639148235</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38">
-        <v>0.009099463932216167</v>
+        <v>0.008795639500021935</v>
       </c>
       <c r="B38">
-        <v>0.009371898137032986</v>
+        <v>0.008625403046607971</v>
       </c>
       <c r="C38">
-        <v>0.00874505378305912</v>
+        <v>0.008063736371695995</v>
       </c>
       <c r="D38">
-        <v>0.009263582527637482</v>
+        <v>0.00828192662447691</v>
       </c>
       <c r="E38">
-        <v>0.009956937283277512</v>
+        <v>0.008261170238256454</v>
       </c>
       <c r="F38">
-        <v>0.009212136268615723</v>
+        <v>0.00613474752753973</v>
       </c>
       <c r="G38">
-        <v>0.006545111071318388</v>
+        <v>0.001585907069966197</v>
       </c>
       <c r="H38">
-        <v>0.005507232621312141</v>
+        <v>0.00163209461607039</v>
       </c>
       <c r="I38">
-        <v>0.008864715695381165</v>
+        <v>0.007010702043771744</v>
       </c>
       <c r="J38">
-        <v>0.01019547693431377</v>
+        <v>0.008549408987164497</v>
       </c>
       <c r="K38">
-        <v>0.00920978095382452</v>
+        <v>0.008661523461341858</v>
       </c>
       <c r="L38">
-        <v>0.01001234352588654</v>
+        <v>0.008782914839684963</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39">
-        <v>0.008837108500301838</v>
+        <v>0.00792646873742342</v>
       </c>
       <c r="B39">
-        <v>0.008825032040476799</v>
+        <v>0.008346583694219589</v>
       </c>
       <c r="C39">
-        <v>0.008586240001022816</v>
+        <v>0.007436528336256742</v>
       </c>
       <c r="D39">
-        <v>0.008792761713266373</v>
+        <v>0.007875699549913406</v>
       </c>
       <c r="E39">
-        <v>0.008942984044551849</v>
+        <v>0.007693808991461992</v>
       </c>
       <c r="F39">
-        <v>0.008375601842999458</v>
+        <v>0.005904713179916143</v>
       </c>
       <c r="G39">
-        <v>0.00463171536102891</v>
+        <v>0.001119242981076241</v>
       </c>
       <c r="H39">
-        <v>0.004457714501768351</v>
+        <v>0.001419718377292156</v>
       </c>
       <c r="I39">
-        <v>0.008157966658473015</v>
+        <v>0.0059238001704216</v>
       </c>
       <c r="J39">
-        <v>0.009997870773077011</v>
+        <v>0.008273917250335217</v>
       </c>
       <c r="K39">
-        <v>0.009166238829493523</v>
+        <v>0.008294889703392982</v>
       </c>
       <c r="L39">
-        <v>0.009700948372483253</v>
+        <v>0.008649615570902824</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40">
-        <v>0.008185033686459064</v>
+        <v>0.007418251130729914</v>
       </c>
       <c r="B40">
-        <v>0.008287000469863415</v>
+        <v>0.007974112406373024</v>
       </c>
       <c r="C40">
-        <v>0.007667024619877338</v>
+        <v>0.007191507611423731</v>
       </c>
       <c r="D40">
-        <v>0.008419496938586235</v>
+        <v>0.007383295800536871</v>
       </c>
       <c r="E40">
-        <v>0.008631521835923195</v>
+        <v>0.007381818257272243</v>
       </c>
       <c r="F40">
-        <v>0.007048069033771753</v>
+        <v>0.004395070485770702</v>
       </c>
       <c r="G40">
-        <v>0.003994588274508715</v>
+        <v>0.0008723610080778599</v>
       </c>
       <c r="H40">
-        <v>0.003972521051764488</v>
+        <v>0.00104310258757323</v>
       </c>
       <c r="I40">
-        <v>0.008091810159385204</v>
+        <v>0.005496886558830738</v>
       </c>
       <c r="J40">
-        <v>0.009464239701628685</v>
+        <v>0.007949790917336941</v>
       </c>
       <c r="K40">
-        <v>0.008665004745125771</v>
+        <v>0.008030611090362072</v>
       </c>
       <c r="L40">
-        <v>0.0086101358756423</v>
+        <v>0.008237455971539021</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41">
-        <v>0.00781644880771637</v>
+        <v>0.007324603386223316</v>
       </c>
       <c r="B41">
-        <v>0.007532502524554729</v>
+        <v>0.007325431797653437</v>
       </c>
       <c r="C41">
-        <v>0.007441720925271511</v>
+        <v>0.006858693901449442</v>
       </c>
       <c r="D41">
-        <v>0.007661668583750725</v>
+        <v>0.006775896996259689</v>
       </c>
       <c r="E41">
-        <v>0.008334657177329063</v>
+        <v>0.00642592366784811</v>
       </c>
       <c r="F41">
-        <v>0.006450464017689228</v>
+        <v>0.004086571745574474</v>
       </c>
       <c r="G41">
-        <v>0.002999757416546345</v>
+        <v>0.0005882037221454084</v>
       </c>
       <c r="H41">
-        <v>0.003759237704798579</v>
+        <v>0.0009042904712259769</v>
       </c>
       <c r="I41">
-        <v>0.005870094057172537</v>
+        <v>0.004223370924592018</v>
       </c>
       <c r="J41">
-        <v>0.009089017286896706</v>
+        <v>0.00731388758867979</v>
       </c>
       <c r="K41">
-        <v>0.007836080156266689</v>
+        <v>0.007234262768179178</v>
       </c>
       <c r="L41">
-        <v>0.007924188859760761</v>
+        <v>0.006859277840703726</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42">
-        <v>1.232081965521101E-17</v>
+        <v>1.172048753538636E-17</v>
       </c>
       <c r="B42">
-        <v>1.596203645162555E-17</v>
+        <v>1.960250795830817E-17</v>
       </c>
       <c r="C42">
-        <v>2.352005022861034E-17</v>
+        <v>6.735712289274909E-18</v>
       </c>
       <c r="D42">
-        <v>2.498063943214217E-18</v>
+        <v>1.976287677238628E-17</v>
       </c>
       <c r="E42">
-        <v>1.427093682679356E-17</v>
+        <v>-8.909353101113685E-18</v>
       </c>
       <c r="F42">
-        <v>5.920245794966551E-18</v>
+        <v>1.226001195402101E-17</v>
       </c>
       <c r="G42">
-        <v>1.529889568070913E-18</v>
+        <v>6.97164115717759E-18</v>
       </c>
       <c r="H42">
-        <v>1.689958632574545E-18</v>
+        <v>-9.553643459845779E-19</v>
       </c>
       <c r="I42">
-        <v>-5.636845858890065E-18</v>
+        <v>3.238709883165622E-17</v>
       </c>
       <c r="J42">
-        <v>3.049156896305727E-18</v>
+        <v>5.144766865830232E-18</v>
       </c>
       <c r="K42">
-        <v>8.531793955139369E-18</v>
+        <v>6.883510439584047E-18</v>
       </c>
       <c r="L42">
-        <v>5.769029527571192E-19</v>
+        <v>2.152607345940839E-17</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43">
-        <v>-1.380078639177251E-17</v>
+        <v>5.770600550349583E-18</v>
       </c>
       <c r="B43">
-        <v>5.831454160063578E-18</v>
+        <v>-7.074554212702916E-19</v>
       </c>
       <c r="C43">
-        <v>1.683705291900251E-17</v>
+        <v>-1.24026278177925E-17</v>
       </c>
       <c r="D43">
-        <v>-3.099170469528337E-17</v>
+        <v>4.188918360693369E-19</v>
       </c>
       <c r="E43">
-        <v>-5.467498929840885E-19</v>
+        <v>-1.691025674885223E-17</v>
       </c>
       <c r="F43">
-        <v>-1.092081233256195E-17</v>
+        <v>-2.842103404322412E-19</v>
       </c>
       <c r="G43">
-        <v>-1.028568320590903E-17</v>
+        <v>1.08520316442427E-18</v>
       </c>
       <c r="H43">
-        <v>-1.140500250411986E-17</v>
+        <v>-2.953873217083193E-17</v>
       </c>
       <c r="I43">
-        <v>-6.140456163279193E-18</v>
+        <v>-5.912577830688185E-18</v>
       </c>
       <c r="J43">
-        <v>-2.759654021669824E-17</v>
+        <v>-1.03155973655814E-17</v>
       </c>
       <c r="K43">
-        <v>-9.465641162042334E-18</v>
+        <v>6.946964705143908E-19</v>
       </c>
       <c r="L43">
-        <v>-3.48644096404821E-18</v>
+        <v>-1.30848574357048E-17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>